<commit_message>
Toevoegen samenvattend tabblad bij tijdsmetingen van de implementatie volgens de paper.
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25300" windowHeight="14560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
     <sheet name="Subsumes2" sheetId="5" r:id="rId2"/>
+    <sheet name="Samenvatting" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Tester</t>
   </si>
@@ -107,18 +118,53 @@
     </r>
   </si>
   <si>
-    <t>subsumes1 =</t>
+    <t>1 netwerk [ns]</t>
+  </si>
+  <si>
+    <t>Subsumes 1</t>
+  </si>
+  <si>
+    <t>Subsumes 2</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k+1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="171" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +218,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -211,20 +287,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -253,18 +327,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+  <cellStyles count="3">
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -277,7 +365,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -319,12 +407,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -354,12 +442,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -566,18 +654,18 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:M22"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,236 +685,236 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <f>15^12</f>
         <v>129746337890625</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>19593210626</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <f>B3/1000000000</f>
         <v>19.593210626000001</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="6">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5">
         <v>19522727046</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
         <v>19.522727046</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="6">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="5">
         <v>19718671932</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>19.718671931999999</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="6">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5">
         <v>19626334392</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>19.626334392</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="6">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5">
         <v>19472517319</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>19.472517319000001</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5">
         <v>19633837384</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f>B8/1000000000</f>
         <v>19.633837384</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="6">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5">
         <v>19473271505</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f>B9/1000000000</f>
         <v>19.473271505</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5">
         <v>20111010358</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <f t="shared" ref="C10:C14" si="1">B10/1000000000</f>
         <v>20.111010358000001</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5">
         <v>19514648451</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <f t="shared" si="1"/>
         <v>19.514648450999999</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
         <v>19553747871</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <f t="shared" si="1"/>
         <v>19.553747870999999</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <f>AVERAGE(B3:B12)</f>
         <v>19621997688.400002</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <f t="shared" si="1"/>
         <v>19.6219976884</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <f>B13/A3</f>
         <v>1.5123353774301645E-4</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <f t="shared" si="1"/>
         <v>1.5123353774301644E-13</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <f>(55^33)</f>
         <v>2.703763826271497E+57</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f>A17*$B$14</f>
         <v>4.0889976866863301E+53</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <f>C14*A17</f>
         <v>4.0889976866863297E+44</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f>C17/(60*60)</f>
         <v>1.1358326907462027E+41</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <f>D17/24</f>
         <v>4.7326362114425111E+39</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f>E17/365</f>
         <v>1.2966126606691812E+37</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -867,7 +955,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -922,19 +1010,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,247 +1042,238 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <f>15^12</f>
         <v>129746337890625</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>14436440266</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <f>B3/1000000000</f>
         <v>14.436440266</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="6">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5">
         <v>14423809895</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
         <v>14.423809895</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="6">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="5">
         <v>14881150749</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>14.881150749</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="6">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5">
         <v>14375324196</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>14.375324195999999</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="6">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5">
         <v>14544453742</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>14.544453742</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5">
         <v>14714846363</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f>B8/1000000000</f>
         <v>14.714846362999999</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="6">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5">
         <v>14688048051</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f>B9/1000000000</f>
         <v>14.688048051000001</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5">
         <v>14346266032</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <f t="shared" ref="C10:C14" si="1">B10/1000000000</f>
         <v>14.346266032000001</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5">
         <v>14582072964</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <f t="shared" si="1"/>
         <v>14.582072964</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
         <v>14436843505</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <f t="shared" si="1"/>
         <v>14.436843505000001</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <f>AVERAGE(B3:B12)</f>
         <v>14542925576.299999</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <f t="shared" si="1"/>
         <v>14.5429255763</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="17">
-        <f>Subsumes1!B13</f>
-        <v>19621997688.400002</v>
-      </c>
-      <c r="H13" s="18">
-        <f>(G13-B13)/B13</f>
-        <v>0.34924693009343011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <f>B13/A3</f>
         <v>1.1208736842005942E-4</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <f t="shared" si="1"/>
         <v>1.1208736842005942E-13</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <f>(55^33)</f>
         <v>2.703763826271497E+57</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f>A17*$B$14</f>
         <v>3.0305777211612283E+53</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <f>C14*A17</f>
         <v>3.0305777211612281E+44</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f>C17/(60*60)</f>
         <v>8.4182714476700783E+40</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <f>D17/24</f>
         <v>3.5076131031958657E+39</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f>E17/365</f>
         <v>9.6098989128653852E+36</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1235,7 +1314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1285,4 +1364,206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="19"/>
+    <col min="6" max="17" width="7.83203125" style="22" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="31" x14ac:dyDescent="0.4">
+      <c r="A2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="20">
+        <f>Subsumes1!B14</f>
+        <v>1.5123353774301645E-4</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="22">
+        <f>Subsumes1!B22</f>
+        <v>15</v>
+      </c>
+      <c r="G2" s="22">
+        <f>Subsumes1!C22</f>
+        <v>15</v>
+      </c>
+      <c r="H2" s="22">
+        <f>Subsumes1!D22</f>
+        <v>45</v>
+      </c>
+      <c r="I2" s="22">
+        <f>Subsumes1!E22</f>
+        <v>105</v>
+      </c>
+      <c r="J2" s="22">
+        <f>Subsumes1!F22</f>
+        <v>255</v>
+      </c>
+      <c r="K2" s="22">
+        <f>Subsumes1!G22</f>
+        <v>540</v>
+      </c>
+      <c r="L2" s="22">
+        <f>Subsumes1!H22</f>
+        <v>795</v>
+      </c>
+      <c r="M2" s="22">
+        <f>Subsumes1!I22</f>
+        <v>795</v>
+      </c>
+      <c r="N2" s="22">
+        <f>Subsumes1!J22</f>
+        <v>660</v>
+      </c>
+      <c r="O2" s="22">
+        <f>Subsumes1!K22</f>
+        <v>345</v>
+      </c>
+      <c r="P2" s="22">
+        <f>Subsumes1!L22</f>
+        <v>120</v>
+      </c>
+      <c r="Q2" s="22">
+        <f>Subsumes1!M22</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="31" x14ac:dyDescent="0.4">
+      <c r="A3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="20">
+        <f>Subsumes2!B14</f>
+        <v>1.1208736842005942E-4</v>
+      </c>
+      <c r="C3" s="21">
+        <f>ABS(B2-B3)/B2</f>
+        <v>0.25884582154968927</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="22">
+        <f>Subsumes2!B22</f>
+        <v>15</v>
+      </c>
+      <c r="G3" s="22">
+        <f>Subsumes2!C22</f>
+        <v>14</v>
+      </c>
+      <c r="H3" s="22">
+        <f>Subsumes2!D22</f>
+        <v>39</v>
+      </c>
+      <c r="I3" s="22">
+        <f>Subsumes2!E22</f>
+        <v>84</v>
+      </c>
+      <c r="J3" s="22">
+        <f>Subsumes2!F22</f>
+        <v>186</v>
+      </c>
+      <c r="K3" s="22">
+        <f>Subsumes2!G22</f>
+        <v>355</v>
+      </c>
+      <c r="L3" s="22">
+        <f>Subsumes2!H22</f>
+        <v>457</v>
+      </c>
+      <c r="M3" s="22">
+        <f>Subsumes2!I22</f>
+        <v>382</v>
+      </c>
+      <c r="N3" s="22">
+        <f>Subsumes2!J22</f>
+        <v>257</v>
+      </c>
+      <c r="O3" s="22">
+        <f>Subsumes2!K22</f>
+        <v>108</v>
+      </c>
+      <c r="P3" s="22">
+        <f>Subsumes2!L22</f>
+        <v>21</v>
+      </c>
+      <c r="Q3" s="22">
+        <f>Subsumes2!M22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="23" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="F4" s="24">
+        <f>ABS(F2-F3)/F2</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
+        <f t="shared" ref="G4:Q4" si="0">ABS(G2-G3)/G2</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="H4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.27058823529411763</v>
+      </c>
+      <c r="K4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.34259259259259262</v>
+      </c>
+      <c r="L4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.42515723270440253</v>
+      </c>
+      <c r="M4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.51949685534591195</v>
+      </c>
+      <c r="N4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.6106060606060606</v>
+      </c>
+      <c r="O4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.68695652173913047</v>
+      </c>
+      <c r="P4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with results for updated implementation + graphical representation
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25300" windowHeight="14560" activeTab="2"/>
+    <workbookView xWindow="1660" yWindow="460" windowWidth="23940" windowHeight="14560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
     <sheet name="Subsumes2" sheetId="5" r:id="rId2"/>
-    <sheet name="Samenvatting" sheetId="6" r:id="rId3"/>
+    <sheet name="Subsumes3" sheetId="7" r:id="rId3"/>
+    <sheet name="Samenvatting" sheetId="6" r:id="rId4"/>
+    <sheet name="Grafiek1" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>Tester</t>
   </si>
@@ -153,6 +155,9 @@
       <t>k+1</t>
     </r>
   </si>
+  <si>
+    <t>Subsumes 3</t>
+  </si>
 </sst>
 </file>
 
@@ -162,7 +167,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -292,7 +297,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,11 +340,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,6 +349,12 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -362,6 +370,873 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-BE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Samenvatting!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 netwerk [ns]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Samenvatting!$A$2:$A$3,Samenvatting!$A$5)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Subsumes 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Subsumes 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Subsumes 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Samenvatting!$B$2:$B$3,Samenvatting!$B$5)</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.000151233537743016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000112087368420059</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000105815333887678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2063041744"/>
+        <c:axId val="-2063036848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2063041744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2063036848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2063036848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2063041744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -686,14 +1561,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -869,14 +1744,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -905,14 +1780,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1010,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1043,14 +1918,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1228,14 +2103,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -1264,14 +2139,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1305,7 +2180,7 @@
         <v>257</v>
       </c>
       <c r="K22">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="L22">
         <v>21</v>
@@ -1368,199 +2243,678 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <f>15^12</f>
+        <v>129746337890625</v>
+      </c>
+      <c r="B3" s="5">
+        <v>13609086846</v>
+      </c>
+      <c r="C3" s="6">
+        <f>B3/1000000000</f>
+        <v>13.609086846</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+      <c r="B4" s="5">
+        <v>14137608017</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
+        <v>14.137608017</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="5">
+        <v>14130587666</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>14.130587666</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="5">
+        <v>13830458357</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>13.830458356999999</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="5">
+        <v>13311338571</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>13.311338571</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5">
+        <v>14849284345</v>
+      </c>
+      <c r="C8" s="6">
+        <f>B8/1000000000</f>
+        <v>14.849284344999999</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5">
+        <v>13711245318</v>
+      </c>
+      <c r="C9" s="6">
+        <f>B9/1000000000</f>
+        <v>13.711245318</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5">
+        <v>13083626478</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ref="C10:C14" si="1">B10/1000000000</f>
+        <v>13.083626477999999</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5">
+        <v>13381515211</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="1"/>
+        <v>13.381515211</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
+        <v>13246769837</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="1"/>
+        <v>13.246769837</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11">
+        <f>AVERAGE(B3:B12)</f>
+        <v>13729152064.6</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="1"/>
+        <v>13.729152064600001</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14">
+        <f>B13/A3</f>
+        <v>1.0581533388767822E-4</v>
+      </c>
+      <c r="C14" s="13">
+        <f t="shared" si="1"/>
+        <v>1.0581533388767823E-13</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <f>(55^33)</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="B17" s="5">
+        <f>A17*$B$14</f>
+        <v>2.8609967203034486E+53</v>
+      </c>
+      <c r="C17" s="5">
+        <f>C14*A17</f>
+        <v>2.860996720303449E+44</v>
+      </c>
+      <c r="D17" s="3">
+        <f>C17/(60*60)</f>
+        <v>7.9472131119540254E+40</v>
+      </c>
+      <c r="E17" s="3">
+        <f>D17/24</f>
+        <v>3.3113387966475108E+39</v>
+      </c>
+      <c r="F17" s="3">
+        <f>E17/365</f>
+        <v>9.0721610867055085E+36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>84</v>
+      </c>
+      <c r="F22">
+        <v>186</v>
+      </c>
+      <c r="G22">
+        <v>355</v>
+      </c>
+      <c r="H22">
+        <v>457</v>
+      </c>
+      <c r="I22">
+        <v>382</v>
+      </c>
+      <c r="J22">
+        <v>257</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>21</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <v>36</v>
+      </c>
+      <c r="G23">
+        <v>53</v>
+      </c>
+      <c r="H23">
+        <v>53</v>
+      </c>
+      <c r="I23">
+        <v>44</v>
+      </c>
+      <c r="J23">
+        <v>23</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A19:F19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" activeCellId="1" sqref="A1:B3 A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="19"/>
-    <col min="6" max="17" width="7.83203125" style="22" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="19"/>
+    <col min="1" max="1" width="17.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="18"/>
+    <col min="7" max="18" width="7.83203125" style="21" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="31" x14ac:dyDescent="0.4">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+      <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <f>Subsumes1!B14</f>
         <v>1.5123353774301645E-4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="22">
+      <c r="G2" s="21">
         <f>Subsumes1!B22</f>
         <v>15</v>
       </c>
-      <c r="G2" s="22">
+      <c r="H2" s="21">
         <f>Subsumes1!C22</f>
         <v>15</v>
       </c>
-      <c r="H2" s="22">
+      <c r="I2" s="21">
         <f>Subsumes1!D22</f>
         <v>45</v>
       </c>
-      <c r="I2" s="22">
+      <c r="J2" s="21">
         <f>Subsumes1!E22</f>
         <v>105</v>
       </c>
-      <c r="J2" s="22">
+      <c r="K2" s="21">
         <f>Subsumes1!F22</f>
         <v>255</v>
       </c>
-      <c r="K2" s="22">
+      <c r="L2" s="21">
         <f>Subsumes1!G22</f>
         <v>540</v>
       </c>
-      <c r="L2" s="22">
+      <c r="M2" s="21">
         <f>Subsumes1!H22</f>
         <v>795</v>
       </c>
-      <c r="M2" s="22">
+      <c r="N2" s="21">
         <f>Subsumes1!I22</f>
         <v>795</v>
       </c>
-      <c r="N2" s="22">
+      <c r="O2" s="21">
         <f>Subsumes1!J22</f>
         <v>660</v>
       </c>
-      <c r="O2" s="22">
+      <c r="P2" s="21">
         <f>Subsumes1!K22</f>
         <v>345</v>
       </c>
-      <c r="P2" s="22">
+      <c r="Q2" s="21">
         <f>Subsumes1!L22</f>
         <v>120</v>
       </c>
-      <c r="Q2" s="22">
+      <c r="R2" s="21">
         <f>Subsumes1!M22</f>
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="31" x14ac:dyDescent="0.4">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <f>Subsumes2!B14</f>
         <v>1.1208736842005942E-4</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <f>ABS(B2-B3)/B2</f>
         <v>0.25884582154968927</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="20"/>
+      <c r="F3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="22">
+      <c r="G3" s="21">
         <f>Subsumes2!B22</f>
         <v>15</v>
       </c>
-      <c r="G3" s="22">
+      <c r="H3" s="21">
         <f>Subsumes2!C22</f>
         <v>14</v>
       </c>
-      <c r="H3" s="22">
+      <c r="I3" s="21">
         <f>Subsumes2!D22</f>
         <v>39</v>
       </c>
-      <c r="I3" s="22">
+      <c r="J3" s="21">
         <f>Subsumes2!E22</f>
         <v>84</v>
       </c>
-      <c r="J3" s="22">
+      <c r="K3" s="21">
         <f>Subsumes2!F22</f>
         <v>186</v>
       </c>
-      <c r="K3" s="22">
+      <c r="L3" s="21">
         <f>Subsumes2!G22</f>
         <v>355</v>
       </c>
-      <c r="L3" s="22">
+      <c r="M3" s="21">
         <f>Subsumes2!H22</f>
         <v>457</v>
       </c>
-      <c r="M3" s="22">
+      <c r="N3" s="21">
         <f>Subsumes2!I22</f>
         <v>382</v>
       </c>
-      <c r="N3" s="22">
+      <c r="O3" s="21">
         <f>Subsumes2!J22</f>
         <v>257</v>
       </c>
-      <c r="O3" s="22">
+      <c r="P3" s="21">
         <f>Subsumes2!K22</f>
-        <v>108</v>
-      </c>
-      <c r="P3" s="22">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="21">
         <f>Subsumes2!L22</f>
         <v>21</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="R3" s="21">
         <f>Subsumes2!M22</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="23" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="F4" s="24">
-        <f>ABS(F2-F3)/F2</f>
+    <row r="4" spans="1:18" s="22" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="G4" s="23">
+        <f>ABS(G2-G3)/G2</f>
         <v>0</v>
       </c>
-      <c r="G4" s="24">
-        <f t="shared" ref="G4:Q4" si="0">ABS(G2-G3)/G2</f>
+      <c r="H4" s="23">
+        <f t="shared" ref="H4:R4" si="0">ABS(H2-H3)/H2</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="H4" s="24">
+      <c r="I4" s="23">
         <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="I4" s="24">
+      <c r="J4" s="23">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="J4" s="24">
+      <c r="K4" s="23">
         <f t="shared" si="0"/>
         <v>0.27058823529411763</v>
       </c>
-      <c r="K4" s="24">
+      <c r="L4" s="23">
         <f t="shared" si="0"/>
         <v>0.34259259259259262</v>
       </c>
-      <c r="L4" s="24">
+      <c r="M4" s="23">
         <f t="shared" si="0"/>
         <v>0.42515723270440253</v>
       </c>
-      <c r="M4" s="24">
+      <c r="N4" s="23">
         <f t="shared" si="0"/>
         <v>0.51949685534591195</v>
       </c>
-      <c r="N4" s="24">
+      <c r="O4" s="23">
         <f t="shared" si="0"/>
         <v>0.6106060606060606</v>
       </c>
-      <c r="O4" s="24">
+      <c r="P4" s="23">
         <f t="shared" si="0"/>
-        <v>0.68695652173913047</v>
-      </c>
-      <c r="P4" s="24">
+        <v>0.71014492753623193</v>
+      </c>
+      <c r="Q4" s="23">
         <f t="shared" si="0"/>
         <v>0.82499999999999996</v>
       </c>
-      <c r="Q4" s="24">
+      <c r="R4" s="23">
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+      <c r="A5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="19">
+        <f>Subsumes3!B14</f>
+        <v>1.0581533388767822E-4</v>
+      </c>
+      <c r="C5" s="20">
+        <f>(B3-B5)/B3</f>
+        <v>5.5956657924879416E-2</v>
+      </c>
+      <c r="D5" s="20">
+        <f>ABS(B2-B5)/B2</f>
+        <v>0.30031833238282835</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="21">
+        <f>Subsumes3!B22</f>
+        <v>15</v>
+      </c>
+      <c r="H5" s="21">
+        <f>Subsumes3!C22</f>
+        <v>14</v>
+      </c>
+      <c r="I5" s="21">
+        <f>Subsumes3!D22</f>
+        <v>39</v>
+      </c>
+      <c r="J5" s="21">
+        <f>Subsumes3!E22</f>
+        <v>84</v>
+      </c>
+      <c r="K5" s="21">
+        <f>Subsumes3!F22</f>
+        <v>186</v>
+      </c>
+      <c r="L5" s="21">
+        <f>Subsumes3!G22</f>
+        <v>355</v>
+      </c>
+      <c r="M5" s="21">
+        <f>Subsumes3!H22</f>
+        <v>457</v>
+      </c>
+      <c r="N5" s="21">
+        <f>Subsumes3!I22</f>
+        <v>382</v>
+      </c>
+      <c r="O5" s="21">
+        <f>Subsumes3!J22</f>
+        <v>257</v>
+      </c>
+      <c r="P5" s="21">
+        <f>Subsumes3!K22</f>
+        <v>100</v>
+      </c>
+      <c r="Q5" s="21">
+        <f>Subsumes3!L22</f>
+        <v>21</v>
+      </c>
+      <c r="R5" s="21">
+        <f>Subsumes3!M22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G6" s="23">
+        <f>ABS(G3-G5)/G3</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="23">
+        <f t="shared" ref="H6:R6" si="1">ABS(H3-H5)/H3</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Toevoegen van tijdsmetingen na het toevoegen van Lemma 4 aan de implementatie
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="460" windowWidth="23940" windowHeight="14560" activeTab="2"/>
+    <workbookView xWindow="4420" yWindow="460" windowWidth="21180" windowHeight="14560" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
     <sheet name="Subsumes2" sheetId="5" r:id="rId2"/>
     <sheet name="Subsumes3" sheetId="7" r:id="rId3"/>
-    <sheet name="Samenvatting" sheetId="6" r:id="rId4"/>
-    <sheet name="Grafiek1" sheetId="8" r:id="rId5"/>
+    <sheet name="Subsumes4" sheetId="9" r:id="rId4"/>
+    <sheet name="Samenvatting" sheetId="6" r:id="rId5"/>
+    <sheet name="Grafiek1" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
   <si>
     <t>Tester</t>
   </si>
@@ -158,6 +159,12 @@
   <si>
     <t>Subsumes 3</t>
   </si>
+  <si>
+    <t>Subsumes 4</t>
+  </si>
+  <si>
+    <t>=&gt; toevoegen van lemma 4</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +176,7 @@
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +260,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -297,7 +312,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,9 +368,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="2" builtinId="3"/>
@@ -512,9 +531,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Samenvatting!$A$2:$A$3,Samenvatting!$A$5)</c:f>
+              <c:f>(Samenvatting!$A$2:$A$3,Samenvatting!$A$5,Samenvatting!$A$7)</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Subsumes 1</c:v>
                 </c:pt>
@@ -524,15 +543,18 @@
                 <c:pt idx="2">
                   <c:v>Subsumes 3</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>Subsumes 4</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Samenvatting!$B$2:$B$3,Samenvatting!$B$5)</c:f>
+              <c:f>(Samenvatting!$B$2:$B$3,Samenvatting!$B$5,Samenvatting!$B$7)</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.000151233537743016</c:v>
                 </c:pt>
@@ -541,6 +563,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.000105815333887678</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.57498343901054E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,11 +581,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2071712752"/>
-        <c:axId val="-2081898400"/>
+        <c:axId val="-2076787552"/>
+        <c:axId val="-2076784400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2071712752"/>
+        <c:axId val="-2076787552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +628,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081898400"/>
+        <c:crossAx val="-2076784400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -611,7 +636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2081898400"/>
+        <c:axId val="-2076784400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +672,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071712752"/>
+        <c:crossAx val="-2076787552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1677,14 +1702,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1860,14 +1885,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -1896,14 +1921,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2034,14 +2059,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2219,14 +2244,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2255,14 +2280,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2361,8 +2386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2394,14 +2419,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2579,14 +2604,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2615,14 +2640,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2719,10 +2744,373 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="H2" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <f>15^12</f>
+        <v>129746337890625</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2067793954</v>
+      </c>
+      <c r="C3" s="6">
+        <f>B3/1000000000</f>
+        <v>2.0677939539999999</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="5">
+        <v>2041149952</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
+        <v>2.041149952</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
+      <c r="B5" s="5">
+        <v>1972292050</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9722920500000001</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" s="5">
+        <v>1937625274</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>1.937625274</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="5">
+        <v>2138018651</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1380186509999999</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5">
+        <v>2006280233</v>
+      </c>
+      <c r="C8" s="6">
+        <f>B8/1000000000</f>
+        <v>2.006280233</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5">
+        <v>2010043796</v>
+      </c>
+      <c r="C9" s="6">
+        <f>B9/1000000000</f>
+        <v>2.0100437960000002</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5">
+        <v>2106993709</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ref="C10:C14" si="1">B10/1000000000</f>
+        <v>2.1069937090000002</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5">
+        <v>2069158799</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="1"/>
+        <v>2.0691587990000002</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
+        <v>2085476927</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="1"/>
+        <v>2.0854769270000002</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11">
+        <f>AVERAGE(B3:B12)</f>
+        <v>2043483334.5</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0434833344999999</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14">
+        <f>B13/A3</f>
+        <v>1.5749834390105394E-5</v>
+      </c>
+      <c r="C14" s="13">
+        <f t="shared" si="1"/>
+        <v>1.5749834390105394E-14</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <f>(55^33)</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="B17" s="5">
+        <f>A17*$B$14</f>
+        <v>4.2583832493733766E+52</v>
+      </c>
+      <c r="C17" s="5">
+        <f>C14*A17</f>
+        <v>4.2583832493733769E+43</v>
+      </c>
+      <c r="D17" s="3">
+        <f>C17/(60*60)</f>
+        <v>1.1828842359370491E+40</v>
+      </c>
+      <c r="E17" s="3">
+        <f>D17/24</f>
+        <v>4.9286843164043711E+38</v>
+      </c>
+      <c r="F17" s="3">
+        <f>E17/365</f>
+        <v>1.3503244702477728E+36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>84</v>
+      </c>
+      <c r="F22">
+        <v>186</v>
+      </c>
+      <c r="G22">
+        <v>355</v>
+      </c>
+      <c r="H22">
+        <v>457</v>
+      </c>
+      <c r="I22">
+        <v>382</v>
+      </c>
+      <c r="J22">
+        <v>257</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>21</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <v>36</v>
+      </c>
+      <c r="G23">
+        <v>53</v>
+      </c>
+      <c r="H23">
+        <v>53</v>
+      </c>
+      <c r="I23">
+        <v>44</v>
+      </c>
+      <c r="J23">
+        <v>23</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A19:F19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" activeCellId="1" sqref="A1:B3 A5:B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -3033,6 +3421,74 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+      <c r="A7" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="19">
+        <f>Subsumes4!B14</f>
+        <v>1.5749834390105394E-5</v>
+      </c>
+      <c r="C7" s="20">
+        <f>(B5-B7)/B5</f>
+        <v>0.85115735298984496</v>
+      </c>
+      <c r="D7" s="20">
+        <f>(B2-B7)/B2</f>
+        <v>0.89585752852738065</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="21">
+        <f>Subsumes4!B22</f>
+        <v>15</v>
+      </c>
+      <c r="H7" s="21">
+        <f>Subsumes4!C22</f>
+        <v>14</v>
+      </c>
+      <c r="I7" s="21">
+        <f>Subsumes4!D22</f>
+        <v>39</v>
+      </c>
+      <c r="J7" s="21">
+        <f>Subsumes4!E22</f>
+        <v>84</v>
+      </c>
+      <c r="K7" s="21">
+        <f>Subsumes4!F22</f>
+        <v>186</v>
+      </c>
+      <c r="L7" s="21">
+        <f>Subsumes4!G22</f>
+        <v>355</v>
+      </c>
+      <c r="M7" s="21">
+        <f>Subsumes4!H22</f>
+        <v>457</v>
+      </c>
+      <c r="N7" s="21">
+        <f>Subsumes4!I22</f>
+        <v>382</v>
+      </c>
+      <c r="O7" s="21">
+        <f>Subsumes4!J22</f>
+        <v>257</v>
+      </c>
+      <c r="P7" s="21">
+        <f>Subsumes4!K22</f>
+        <v>100</v>
+      </c>
+      <c r="Q7" s="21">
+        <f>Subsumes4!L22</f>
+        <v>21</v>
+      </c>
+      <c r="R7" s="21">
+        <f>Subsumes4!M22</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Toevoegen van de resultaten 7 kanalen 16 comparatoren
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="460" windowWidth="21180" windowHeight="14560" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="4420" yWindow="460" windowWidth="21180" windowHeight="14560" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
   <si>
     <t>Tester</t>
   </si>
@@ -163,7 +163,67 @@
     <t>Subsumes 4</t>
   </si>
   <si>
-    <t>=&gt; toevoegen van lemma 4</t>
+    <t>Subsumes + Redundant Comparators + Lemma 4</t>
+  </si>
+  <si>
+    <t>7 channels, 16 comparators: 1,29E14 networks</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k+1</t>
+    </r>
+  </si>
+  <si>
+    <t>[min]</t>
   </si>
 </sst>
 </file>
@@ -176,9 +236,16 @@
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -262,8 +329,24 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -309,26 +392,26 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -352,29 +435,64 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="2" builtinId="3"/>
@@ -581,11 +699,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2076787552"/>
-        <c:axId val="-2076784400"/>
+        <c:axId val="-2127551360"/>
+        <c:axId val="-2127549904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2076787552"/>
+        <c:axId val="-2127551360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +746,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076784400"/>
+        <c:crossAx val="-2127549904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -636,7 +754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076784400"/>
+        <c:axId val="-2127549904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,7 +790,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076787552"/>
+        <c:crossAx val="-2127551360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2026,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -2744,22 +2862,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="28"/>
+    <col min="15" max="15" width="12.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="28" customWidth="1"/>
+    <col min="19" max="19" width="9.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" style="28" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2777,8 +2905,29 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="O1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
@@ -2787,186 +2936,340 @@
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
-      <c r="H2" s="27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H2" s="29"/>
+      <c r="O2" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <f>15^12</f>
         <v>129746337890625</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="30">
         <v>2067793954</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="31">
         <f>B3/1000000000</f>
         <v>2.0677939539999999</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="O3" s="4">
+        <f>21^16</f>
+        <v>1.4305686902419853E+21</v>
+      </c>
+      <c r="P3" s="30">
+        <v>1352402328845</v>
+      </c>
+      <c r="Q3" s="31">
+        <f>P3/1000000000</f>
+        <v>1352.4023288450001</v>
+      </c>
+      <c r="R3" s="31"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
-      <c r="B4" s="5">
+      <c r="B4" s="30">
         <v>2041149952</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="31">
         <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
         <v>2.041149952</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="31">
+        <f t="shared" ref="Q4:Q7" si="1">P4/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="31"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
-      <c r="B5" s="5">
+      <c r="B5" s="30">
         <v>1972292050</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="31">
         <f t="shared" si="0"/>
         <v>1.9722920500000001</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="31"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="24"/>
-      <c r="B6" s="5">
+      <c r="B6" s="30">
         <v>1937625274</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="31">
         <f t="shared" si="0"/>
         <v>1.937625274</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="31"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="24"/>
-      <c r="B7" s="5">
+      <c r="B7" s="30">
         <v>2138018651</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="31">
         <f t="shared" si="0"/>
         <v>2.1380186509999999</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="31"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="32"/>
+      <c r="B8" s="30">
         <v>2006280233</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="31">
         <f>B8/1000000000</f>
         <v>2.006280233</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="31">
+        <f>P8/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="31"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="32"/>
+      <c r="B9" s="30">
         <v>2010043796</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="31">
         <f>B9/1000000000</f>
         <v>2.0100437960000002</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31">
+        <f>P9/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="31"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="30">
         <v>2106993709</v>
       </c>
-      <c r="C10" s="6">
-        <f t="shared" ref="C10:C14" si="1">B10/1000000000</f>
+      <c r="C10" s="31">
+        <f t="shared" ref="C10:C14" si="2">B10/1000000000</f>
         <v>2.1069937090000002</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5">
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="31">
+        <f t="shared" ref="Q10:Q14" si="3">P10/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="31"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="32"/>
+      <c r="B11" s="30">
         <v>2069158799</v>
       </c>
-      <c r="C11" s="6">
-        <f t="shared" si="1"/>
+      <c r="C11" s="31">
+        <f t="shared" si="2"/>
         <v>2.0691587990000002</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9">
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="31"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" s="34">
         <v>2085476927</v>
       </c>
-      <c r="C12" s="10">
-        <f t="shared" si="1"/>
+      <c r="C12" s="35">
+        <f t="shared" si="2"/>
         <v>2.0854769270000002</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="37"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="36">
         <f>AVERAGE(B3:B12)</f>
         <v>2043483334.5</v>
       </c>
-      <c r="C13" s="12">
-        <f t="shared" si="1"/>
+      <c r="C13" s="37">
+        <f t="shared" si="2"/>
         <v>2.0434833344999999</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="O13" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="36">
+        <f>AVERAGE(P3:P12)</f>
+        <v>1352402328845</v>
+      </c>
+      <c r="Q13" s="37">
+        <f t="shared" si="3"/>
+        <v>1352.4023288450001</v>
+      </c>
+      <c r="R13" s="37">
+        <f>Q13/60</f>
+        <v>22.540038814083335</v>
+      </c>
+      <c r="S13" s="37">
+        <f>R13/60</f>
+        <v>0.37566731356805561</v>
+      </c>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="40">
         <f>B13/A3</f>
         <v>1.5749834390105394E-5</v>
       </c>
-      <c r="C14" s="13">
-        <f t="shared" si="1"/>
+      <c r="C14" s="41">
+        <f t="shared" si="2"/>
         <v>1.5749834390105394E-14</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="O14" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14" s="40">
+        <f>P13/O3</f>
+        <v>9.4535993837264588E-10</v>
+      </c>
+      <c r="Q14" s="41">
+        <f t="shared" si="3"/>
+        <v>9.4535993837264579E-19</v>
+      </c>
+      <c r="R14" s="41">
+        <f>Q14/60</f>
+        <v>1.575599897287743E-20</v>
+      </c>
+      <c r="S14" s="32">
+        <f>R14/60</f>
+        <v>2.6259998288129051E-22</v>
+      </c>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="32"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>8</v>
       </c>
@@ -2976,129 +3279,130 @@
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <f>(55^33)</f>
         <v>2.703763826271497E+57</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="30">
         <f>A17*$B$14</f>
         <v>4.2583832493733766E+52</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="30">
         <f>C14*A17</f>
         <v>4.2583832493733769E+43</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="32">
         <f>C17/(60*60)</f>
         <v>1.1828842359370491E+40</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="32">
         <f>D17/24</f>
         <v>4.9286843164043711E+38</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="32">
         <f>E17/365</f>
         <v>1.3503244702477728E+36</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22">
+      <c r="A19" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="22" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="28">
         <v>15</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="28">
         <v>14</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="28">
         <v>39</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="28">
         <v>84</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="28">
         <v>186</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="28">
         <v>355</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="28">
         <v>457</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="28">
         <v>382</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="28">
         <v>257</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="28">
         <v>100</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="28">
         <v>21</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="28">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23">
+    <row r="23" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="28">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="28">
         <v>3</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="28">
         <v>7</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="28">
         <v>17</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="28">
         <v>36</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="28">
         <v>53</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="28">
         <v>53</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="28">
         <v>44</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="28">
         <v>23</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="28">
         <v>8</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="28">
         <v>4</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="28">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A19:F19"/>
+    <mergeCell ref="O2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated with time measurements for new implementation of array’s
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="460" windowWidth="21180" windowHeight="14560" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="15400" yWindow="460" windowWidth="10000" windowHeight="14560" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
     <sheet name="Subsumes2" sheetId="5" r:id="rId2"/>
     <sheet name="Subsumes3" sheetId="7" r:id="rId3"/>
     <sheet name="Subsumes4" sheetId="9" r:id="rId4"/>
-    <sheet name="Samenvatting" sheetId="6" r:id="rId5"/>
-    <sheet name="Grafiek1" sheetId="8" r:id="rId6"/>
+    <sheet name="Subsumes5" sheetId="10" r:id="rId5"/>
+    <sheet name="Samenvatting" sheetId="6" r:id="rId6"/>
+    <sheet name="Grafiek1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
   <si>
     <t>Tester</t>
   </si>
@@ -225,18 +226,23 @@
   <si>
     <t>[min]</t>
   </si>
+  <si>
+    <t>Subsumes 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,8 +357,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +390,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,12 +418,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -451,12 +481,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,11 +514,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Komma" xfId="2" builtinId="3"/>
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -649,9 +693,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Samenvatting!$A$2:$A$3,Samenvatting!$A$5,Samenvatting!$A$7)</c:f>
+              <c:f>(Samenvatting!$A$2:$A$3,Samenvatting!$A$5,Samenvatting!$A$7,Samenvatting!$A$9)</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Subsumes 1</c:v>
                 </c:pt>
@@ -664,15 +708,18 @@
                 <c:pt idx="3">
                   <c:v>Subsumes 4</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Subsumes 5</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Samenvatting!$B$2:$B$3,Samenvatting!$B$5,Samenvatting!$B$7)</c:f>
+              <c:f>(Samenvatting!$B$2:$B$3,Samenvatting!$B$5,Samenvatting!$B$7,Samenvatting!$B$9)</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.000151233537743016</c:v>
                 </c:pt>
@@ -684,6 +731,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.57498343901054E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5487632479415E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,11 +749,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2127551360"/>
-        <c:axId val="-2127549904"/>
+        <c:axId val="-2027180000"/>
+        <c:axId val="-2030522736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127551360"/>
+        <c:axId val="-2027180000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +796,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127549904"/>
+        <c:crossAx val="-2030522736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -754,7 +804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127549904"/>
+        <c:axId val="-2030522736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,7 +840,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127551360"/>
+        <c:crossAx val="-2027180000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1475,7 +1525,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9321101" cy="6082018"/>
+    <xdr:ext cx="9307763" cy="6065921"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -1820,14 +1870,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2003,14 +2053,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2039,14 +2089,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2144,7 +2194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -2177,14 +2227,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2362,14 +2412,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2398,14 +2448,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2537,14 +2587,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2722,14 +2772,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2758,14 +2808,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2864,30 +2914,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" style="28"/>
-    <col min="15" max="15" width="12.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="28" customWidth="1"/>
-    <col min="19" max="19" width="9.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6" style="28" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="28"/>
+    <col min="1" max="1" width="12.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="26"/>
+    <col min="15" max="15" width="12.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="26" customWidth="1"/>
+    <col min="19" max="19" width="9.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2905,7 +2955,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -2928,472 +2978,485 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="H2" s="29"/>
-      <c r="O2" s="25" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="H2" s="27"/>
+      <c r="O2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <f>15^12</f>
         <v>129746337890625</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="28">
         <v>2067793954</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="29">
         <f>B3/1000000000</f>
         <v>2.0677939539999999</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="O3" s="4">
         <f>21^16</f>
         <v>1.4305686902419853E+21</v>
       </c>
-      <c r="P3" s="30">
+      <c r="P3" s="41">
         <v>1352402328845</v>
       </c>
-      <c r="Q3" s="31">
+      <c r="Q3" s="29">
         <f>P3/1000000000</f>
         <v>1352.4023288450001</v>
       </c>
-      <c r="R3" s="31"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
+      <c r="R3" s="29">
+        <f>Q3/60</f>
+        <v>22.540038814083335</v>
+      </c>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
-      <c r="B4" s="30">
+      <c r="B4" s="28">
         <v>2041149952</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="29">
         <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
         <v>2.041149952</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
       <c r="O4" s="24"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="31">
+      <c r="P4" s="41">
+        <v>1362813541472</v>
+      </c>
+      <c r="Q4" s="29">
         <f t="shared" ref="Q4:Q7" si="1">P4/1000000000</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
+        <v>1362.813541472</v>
+      </c>
+      <c r="R4" s="29">
+        <f>Q4/60</f>
+        <v>22.713559024533332</v>
+      </c>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>1972292050</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <f t="shared" si="0"/>
         <v>1.9722920500000001</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="O5" s="24"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="31">
+      <c r="P5" s="41">
+        <v>1379910665658</v>
+      </c>
+      <c r="Q5" s="29">
+        <f t="shared" si="1"/>
+        <v>1379.910665658</v>
+      </c>
+      <c r="R5" s="29">
+        <f>Q5/60</f>
+        <v>22.9985110943</v>
+      </c>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" s="28">
+        <v>1937625274</v>
+      </c>
+      <c r="C6" s="29">
+        <f t="shared" si="0"/>
+        <v>1.937625274</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="30">
-        <v>1937625274</v>
-      </c>
-      <c r="C6" s="31">
+      <c r="R6" s="29"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="28">
+        <v>2138018651</v>
+      </c>
+      <c r="C7" s="29">
         <f t="shared" si="0"/>
-        <v>1.937625274</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="31">
+        <v>2.1380186509999999</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="30">
-        <v>2138018651</v>
-      </c>
-      <c r="C7" s="31">
-        <f t="shared" si="0"/>
-        <v>2.1380186509999999</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="31"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
-      <c r="B8" s="30">
+      <c r="A8" s="30"/>
+      <c r="B8" s="28">
         <v>2006280233</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="29">
         <f>B8/1000000000</f>
         <v>2.006280233</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="31">
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="29">
         <f>P8/1000000000</f>
         <v>0</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="30"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
-      <c r="B9" s="30">
+      <c r="A9" s="30"/>
+      <c r="B9" s="28">
         <v>2010043796</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="29">
         <f>B9/1000000000</f>
         <v>2.0100437960000002</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="31">
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="29">
         <f>P9/1000000000</f>
         <v>0</v>
       </c>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="30">
+      <c r="A10" s="30"/>
+      <c r="B10" s="28">
         <v>2106993709</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <f t="shared" ref="C10:C14" si="2">B10/1000000000</f>
         <v>2.1069937090000002</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="31">
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="29">
         <f t="shared" ref="Q10:Q14" si="3">P10/1000000000</f>
         <v>0</v>
       </c>
-      <c r="R10" s="31"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
-      <c r="B11" s="30">
+      <c r="A11" s="30"/>
+      <c r="B11" s="28">
         <v>2069158799</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="29">
         <f t="shared" si="2"/>
         <v>2.0691587990000002</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="31">
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R11" s="31"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34">
+      <c r="A12" s="31"/>
+      <c r="B12" s="32">
         <v>2085476927</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="33">
         <f t="shared" si="2"/>
         <v>2.0854769270000002</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="35">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R12" s="37"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="34">
         <f>AVERAGE(B3:B12)</f>
         <v>2043483334.5</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="35">
         <f t="shared" si="2"/>
         <v>2.0434833344999999</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="39"/>
-      <c r="O13" s="32" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+      <c r="O13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="36">
+      <c r="P13" s="34">
         <f>AVERAGE(P3:P12)</f>
-        <v>1352402328845</v>
-      </c>
-      <c r="Q13" s="37">
+        <v>1365042178658.3333</v>
+      </c>
+      <c r="Q13" s="35">
         <f t="shared" si="3"/>
-        <v>1352.4023288450001</v>
-      </c>
-      <c r="R13" s="37">
+        <v>1365.0421786583333</v>
+      </c>
+      <c r="R13" s="35">
         <f>Q13/60</f>
-        <v>22.540038814083335</v>
-      </c>
-      <c r="S13" s="37">
+        <v>22.750702977638888</v>
+      </c>
+      <c r="S13" s="35">
         <f>R13/60</f>
-        <v>0.37566731356805561</v>
-      </c>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
+        <v>0.37917838296064815</v>
+      </c>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="38">
         <f>B13/A3</f>
         <v>1.5749834390105394E-5</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="39">
         <f t="shared" si="2"/>
         <v>1.5749834390105394E-14</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="O14" s="32" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="O14" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="P14" s="40">
+      <c r="P14" s="41">
         <f>P13/O3</f>
-        <v>9.4535993837264588E-10</v>
-      </c>
-      <c r="Q14" s="41">
+        <v>9.5419548041935121E-10</v>
+      </c>
+      <c r="Q14" s="39">
         <f t="shared" si="3"/>
-        <v>9.4535993837264579E-19</v>
-      </c>
-      <c r="R14" s="41">
+        <v>9.5419548041935123E-19</v>
+      </c>
+      <c r="R14" s="39">
         <f>Q14/60</f>
-        <v>1.575599897287743E-20</v>
-      </c>
-      <c r="S14" s="32">
+        <v>1.5903258006989187E-20</v>
+      </c>
+      <c r="S14" s="30">
         <f>R14/60</f>
-        <v>2.6259998288129051E-22</v>
-      </c>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
+        <v>2.6505430011648645E-22</v>
+      </c>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <f>(55^33)</f>
         <v>2.703763826271497E+57</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="28">
         <f>A17*$B$14</f>
         <v>4.2583832493733766E+52</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="28">
         <f>C14*A17</f>
         <v>4.2583832493733769E+43</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="30">
         <f>C17/(60*60)</f>
         <v>1.1828842359370491E+40</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="30">
         <f>D17/24</f>
         <v>4.9286843164043711E+38</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="30">
         <f>E17/365</f>
         <v>1.3503244702477728E+36</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
     </row>
     <row r="22" spans="1:13" ht="20" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="26">
         <v>15</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="26">
         <v>14</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="26">
         <v>39</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E22" s="26">
         <v>84</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="26">
         <v>186</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="26">
         <v>355</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22" s="26">
         <v>457</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="26">
         <v>382</v>
       </c>
-      <c r="J22" s="28">
+      <c r="J22" s="26">
         <v>257</v>
       </c>
-      <c r="K22" s="28">
+      <c r="K22" s="26">
         <v>100</v>
       </c>
-      <c r="L22" s="28">
+      <c r="L22" s="26">
         <v>21</v>
       </c>
-      <c r="M22" s="28">
+      <c r="M22" s="26">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="20" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="26">
         <v>1</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="26">
         <v>3</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="26">
         <v>7</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="26">
         <v>17</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="26">
         <v>36</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G23" s="26">
         <v>53</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="26">
         <v>53</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="26">
         <v>44</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23" s="26">
         <v>23</v>
       </c>
-      <c r="K23" s="28">
+      <c r="K23" s="26">
         <v>8</v>
       </c>
-      <c r="L23" s="28">
+      <c r="L23" s="26">
         <v>4</v>
       </c>
-      <c r="M23" s="28">
+      <c r="M23" s="26">
         <v>1</v>
       </c>
     </row>
@@ -3411,10 +3474,725 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" style="46" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" style="46" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="H2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="O2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+    </row>
+    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <f>15^12</f>
+        <v>129746337890625</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2023124587</v>
+      </c>
+      <c r="C3" s="6">
+        <f>B3/1000000000</f>
+        <v>2.0231245869999999</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="4">
+        <f>15^12</f>
+        <v>129746337890625</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2014121234</v>
+      </c>
+      <c r="J3" s="6">
+        <f>I3/1000000000</f>
+        <v>2.0141212340000001</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="4">
+        <f>15^12</f>
+        <v>129746337890625</v>
+      </c>
+      <c r="P3" s="5">
+        <v>1993895166</v>
+      </c>
+      <c r="Q3" s="6">
+        <f>P3/1000000000</f>
+        <v>1.9938951659999999</v>
+      </c>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="40"/>
+      <c r="B4" s="5">
+        <v>2002377168</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
+        <v>2.0023771680000002</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="5">
+        <v>2000572596</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" ref="J4:J7" si="1">I4/1000000000</f>
+        <v>2.000572596</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="5">
+        <v>1981253500</v>
+      </c>
+      <c r="Q4" s="6">
+        <f t="shared" ref="Q4:Q7" si="2">P4/1000000000</f>
+        <v>1.9812535</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="40"/>
+      <c r="B5" s="5">
+        <v>2060473530</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.0604735299999999</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="5">
+        <v>2050902972</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="1"/>
+        <v>2.0509029719999998</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="5">
+        <v>1985287903</v>
+      </c>
+      <c r="Q5" s="6">
+        <f t="shared" si="2"/>
+        <v>1.9852879029999999</v>
+      </c>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="40"/>
+      <c r="B6" s="5">
+        <v>2022429410</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>2.02242941</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="5">
+        <v>2011235234</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="1"/>
+        <v>2.0112352339999999</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="5">
+        <v>1974888815</v>
+      </c>
+      <c r="Q6" s="6">
+        <f t="shared" si="2"/>
+        <v>1.9748888149999999</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="40"/>
+      <c r="B7" s="5">
+        <v>2034583018</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>2.0345830180000002</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="5">
+        <v>2017898357</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="1"/>
+        <v>2.017898357</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="5">
+        <v>2051868599</v>
+      </c>
+      <c r="Q7" s="6">
+        <f t="shared" si="2"/>
+        <v>2.0518685990000001</v>
+      </c>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5">
+        <v>2030261972</v>
+      </c>
+      <c r="C8" s="6">
+        <f>B8/1000000000</f>
+        <v>2.0302619719999999</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="5">
+        <v>2019170389</v>
+      </c>
+      <c r="J8" s="6">
+        <f>I8/1000000000</f>
+        <v>2.0191703890000001</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="5">
+        <v>2046474795</v>
+      </c>
+      <c r="Q8" s="6">
+        <f>P8/1000000000</f>
+        <v>2.046474795</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5">
+        <v>2046274152</v>
+      </c>
+      <c r="C9" s="6">
+        <f>B9/1000000000</f>
+        <v>2.0462741520000001</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="5">
+        <v>2080879782</v>
+      </c>
+      <c r="J9" s="6">
+        <f>I9/1000000000</f>
+        <v>2.0808797819999998</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="5">
+        <v>1998765277</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>P9/1000000000</f>
+        <v>1.998765277</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5">
+        <v>2032415048</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ref="C10:C14" si="3">B10/1000000000</f>
+        <v>2.0324150479999998</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5">
+        <v>2003218157</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" ref="J10:J14" si="4">I10/1000000000</f>
+        <v>2.0032181570000001</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="5">
+        <v>2045554027</v>
+      </c>
+      <c r="Q10" s="6">
+        <f t="shared" ref="Q10:Q14" si="5">P10/1000000000</f>
+        <v>2.0455540270000001</v>
+      </c>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5">
+        <v>2038092347</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="3"/>
+        <v>2.0380923470000001</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5">
+        <v>2007263862</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="4"/>
+        <v>2.0072638619999998</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="5">
+        <v>2002554271</v>
+      </c>
+      <c r="Q11" s="6">
+        <f t="shared" si="5"/>
+        <v>2.0025542710000002</v>
+      </c>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
+        <v>2038203928</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="3"/>
+        <v>2.0382039280000002</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9">
+        <v>2019682188</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="4"/>
+        <v>2.019682188</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9">
+        <v>2014093615</v>
+      </c>
+      <c r="Q12" s="10">
+        <f t="shared" si="5"/>
+        <v>2.0140936150000002</v>
+      </c>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11">
+        <f>AVERAGE(B3:B12)</f>
+        <v>2032823516</v>
+      </c>
+      <c r="C13" s="12">
+        <f>B13/1000000000</f>
+        <v>2.0328235160000001</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="11">
+        <f>AVERAGE(I3:I12)</f>
+        <v>2022494477.0999999</v>
+      </c>
+      <c r="J13" s="12">
+        <f t="shared" si="4"/>
+        <v>2.0224944771</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="O13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="11">
+        <f>AVERAGE(P3:P12)</f>
+        <v>2009463596.8</v>
+      </c>
+      <c r="Q13" s="12">
+        <f t="shared" si="5"/>
+        <v>2.0094635967999999</v>
+      </c>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14">
+        <f>B13/A3</f>
+        <v>1.5667675473920905E-5</v>
+      </c>
+      <c r="C14" s="13">
+        <f t="shared" si="3"/>
+        <v>1.5667675473920905E-14</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="14">
+        <f>I13/H3</f>
+        <v>1.5588065990771506E-5</v>
+      </c>
+      <c r="J14" s="13">
+        <f t="shared" si="4"/>
+        <v>1.5588065990771505E-14</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="O14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14" s="14">
+        <f>P13/O3</f>
+        <v>1.5487632479415025E-5</v>
+      </c>
+      <c r="Q14" s="13">
+        <f t="shared" si="5"/>
+        <v>1.5487632479415024E-14</v>
+      </c>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="H16" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="O16" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
+    </row>
+    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <f>(55^33)</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="B17" s="5">
+        <f>A17*$B$14</f>
+        <v>4.2361694188148476E+52</v>
+      </c>
+      <c r="C17" s="5">
+        <f>C14*A17</f>
+        <v>4.2361694188148475E+43</v>
+      </c>
+      <c r="D17" s="3">
+        <f>C17/(60*60)</f>
+        <v>1.1767137274485688E+40</v>
+      </c>
+      <c r="E17" s="3">
+        <f>D17/24</f>
+        <v>4.9029738643690367E+38</v>
+      </c>
+      <c r="F17" s="3">
+        <f>E17/365</f>
+        <v>1.3432805107860374E+36</v>
+      </c>
+      <c r="H17" s="4">
+        <f>(55^33)</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="I17" s="5">
+        <f>H17*$B$14</f>
+        <v>4.2361694188148476E+52</v>
+      </c>
+      <c r="J17" s="5">
+        <f>J14*H17</f>
+        <v>4.2146448947380957E+43</v>
+      </c>
+      <c r="K17" s="3">
+        <f>J17/(60*60)</f>
+        <v>1.1707346929828042E+40</v>
+      </c>
+      <c r="L17" s="3">
+        <f>K17/24</f>
+        <v>4.8780612207616843E+38</v>
+      </c>
+      <c r="M17" s="3">
+        <f>L17/365</f>
+        <v>1.3364551289758039E+36</v>
+      </c>
+      <c r="O17" s="4">
+        <f>(55^33)</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="P17" s="5">
+        <f>O17*$B$14</f>
+        <v>4.2361694188148476E+52</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>Q14*O17</f>
+        <v>4.1874900452429877E+43</v>
+      </c>
+      <c r="R17" s="3">
+        <f>Q17/(60*60)</f>
+        <v>1.1631916792341632E+40</v>
+      </c>
+      <c r="S17" s="3">
+        <f>R17/24</f>
+        <v>4.8466319968090131E+38</v>
+      </c>
+      <c r="T17" s="3">
+        <f>S17/365</f>
+        <v>1.3278443826874009E+36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I20" s="48">
+        <f>(B14-I14)/B14</f>
+        <v>5.0811291874094475E-3</v>
+      </c>
+      <c r="P20" s="48">
+        <f>(B14-P14)/B14</f>
+        <v>1.1491366080792502E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P21" s="48">
+        <f>(I14-P14)/I14</f>
+        <v>6.4429744790623529E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="O16:T16"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I14 B14 P14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -3675,7 +4453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="22" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G6" s="23">
         <f>ABS(G3-G5)/G3</f>
         <v>0</v>
@@ -3791,6 +4569,73 @@
       <c r="R7" s="21">
         <f>Subsumes4!M22</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="22" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="G8" s="23">
+        <f>ABS(G5-G7)/G5</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="23">
+        <f t="shared" ref="H8:R8" si="2">ABS(H5-H7)/H5</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="19">
+        <f>MIN(Subsumes5!B14,Subsumes5!I14,Subsumes5!P14)</f>
+        <v>1.5487632479415025E-5</v>
+      </c>
+      <c r="C9" s="20">
+        <f>(B7-B9)/B7</f>
+        <v>1.6647915412691134E-2</v>
+      </c>
+      <c r="D9" s="20">
+        <f>(B2-B9)/B2</f>
+        <v>0.89759128358332552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added time measurements + test run 8 channels, till 5 comps
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="460" windowWidth="10000" windowHeight="14560" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="1840" yWindow="460" windowWidth="23560" windowHeight="14560" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="29">
   <si>
     <t>Tester</t>
   </si>
@@ -229,6 +229,15 @@
   <si>
     <t>Subsumes 5</t>
   </si>
+  <si>
+    <t>Subsumes 6</t>
+  </si>
+  <si>
+    <t>Subsumes 7</t>
+  </si>
+  <si>
+    <t>Subsumes 8</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +249,7 @@
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="170" formatCode="0.0000%"/>
+    <numFmt numFmtId="168" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -523,6 +532,9 @@
     <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -532,9 +544,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -749,11 +758,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2027180000"/>
-        <c:axId val="-2030522736"/>
+        <c:axId val="2130028224"/>
+        <c:axId val="2098277056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2027180000"/>
+        <c:axId val="2130028224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,7 +805,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2030522736"/>
+        <c:crossAx val="2098277056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -804,7 +813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2030522736"/>
+        <c:axId val="2098277056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,11 +845,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027180000"/>
+        <c:crossAx val="2130028224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1514,7 +1523,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1525,7 +1534,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307763" cy="6065921"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -1838,15 +1847,16 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1870,14 +1880,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2053,14 +2063,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2089,14 +2099,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2195,15 +2205,18 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2227,14 +2240,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2412,14 +2425,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2448,14 +2461,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2555,15 +2568,17 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2587,14 +2602,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -2772,14 +2787,14 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -2808,14 +2823,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2914,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2928,9 +2943,7 @@
     <col min="14" max="14" width="8.83203125" style="26"/>
     <col min="15" max="15" width="12.5" style="26" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="26" customWidth="1"/>
-    <col min="19" max="19" width="9.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" style="26" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.5" style="26" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="8.83203125" style="26"/>
@@ -2978,24 +2991,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="H2" s="27"/>
-      <c r="O2" s="43" t="s">
+      <c r="O2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -3333,14 +3346,14 @@
       <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -3369,14 +3382,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
     </row>
     <row r="22" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
@@ -3476,7 +3489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
@@ -3485,11 +3498,11 @@
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" style="46" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" style="43" customWidth="1"/>
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.83203125" style="46" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" style="43" customWidth="1"/>
     <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="20" width="8" bestFit="1" customWidth="1"/>
@@ -3552,30 +3565,30 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="H2" s="43" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="H2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="O2" s="43" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="O2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
     </row>
     <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -3951,7 +3964,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="47"/>
+      <c r="G13" s="44"/>
       <c r="H13" s="3" t="s">
         <v>6</v>
       </c>
@@ -4046,30 +4059,30 @@
       <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="H16" s="43" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="O16" s="43" t="s">
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="O16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
     </row>
     <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -4146,17 +4159,17 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="I20" s="48">
+      <c r="I20" s="45">
         <f>(B14-I14)/B14</f>
         <v>5.0811291874094475E-3</v>
       </c>
-      <c r="P20" s="48">
+      <c r="P20" s="45">
         <f>(B14-P14)/B14</f>
         <v>1.1491366080792502E-2</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P21" s="48">
+      <c r="P21" s="45">
         <f>(I14-P14)/I14</f>
         <v>6.4429744790623529E-3</v>
       </c>
@@ -4189,10 +4202,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -4279,7 +4292,7 @@
         <v>1.1208736842005942E-4</v>
       </c>
       <c r="C3" s="20">
-        <f>ABS(B2-B3)/B2</f>
+        <f>(B2-B3)/B2</f>
         <v>0.25884582154968927</v>
       </c>
       <c r="D3" s="20"/>
@@ -4637,6 +4650,22 @@
         <f>(B2-B9)/B2</f>
         <v>0.89759128358332552</v>
       </c>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Time tests (subsumes7)
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Samenvatting_7" sheetId="12" r:id="rId9"/>
     <sheet name="Grafiek6" sheetId="8" r:id="rId10"/>
     <sheet name="Grafiek7" sheetId="13" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="38">
   <si>
     <t>Tester</t>
   </si>
@@ -194,6 +195,27 @@
   </si>
   <si>
     <t>Subsumes + Redundant Comparators + Permutation optilmalisation + Lemma 4 + test array/hash/… + Lemma 5 + Lemma 6</t>
+  </si>
+  <si>
+    <t>2 kanalen</t>
+  </si>
+  <si>
+    <t>3 kanalen</t>
+  </si>
+  <si>
+    <t>4 kanalen</t>
+  </si>
+  <si>
+    <t>5 kanalen</t>
+  </si>
+  <si>
+    <t>6 kanalen</t>
+  </si>
+  <si>
+    <t>7 kanalen</t>
+  </si>
+  <si>
+    <t>Subsumes7</t>
   </si>
 </sst>
 </file>
@@ -362,7 +384,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -436,6 +458,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -648,8 +677,8 @@
                 <c:pt idx="5">
                   <c:v>1.1599135462834068E-6</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0</c:v>
+                <c:pt idx="6">
+                  <c:v>1.3247841965674459E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -665,11 +694,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="36354688"/>
-        <c:axId val="89327104"/>
+        <c:axId val="75999872"/>
+        <c:axId val="78779904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="36354688"/>
+        <c:axId val="75999872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +741,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89327104"/>
+        <c:crossAx val="78779904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -720,7 +749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89327104"/>
+        <c:axId val="78779904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +812,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36354688"/>
+        <c:crossAx val="75999872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1007,14 +1036,14 @@
               <c:numCache>
                 <c:formatCode>0.0000000E+00</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
                   <c:v>9.5419548041935121E-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.7567906277502009E-11</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2.0264705407886594E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1030,11 +1059,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="89367296"/>
-        <c:axId val="89369984"/>
+        <c:axId val="84308736"/>
+        <c:axId val="84311424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89367296"/>
+        <c:axId val="84308736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,7 +1106,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89369984"/>
+        <c:crossAx val="84311424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1085,7 +1114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89369984"/>
+        <c:axId val="84311424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1177,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89367296"/>
+        <c:crossAx val="84308736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3056,7 +3085,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
     </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -3097,7 +3126,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -3143,6 +3172,155 @@
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A19:F19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>16093076</v>
+      </c>
+      <c r="C3">
+        <v>20097184</v>
+      </c>
+      <c r="D3">
+        <v>19914673</v>
+      </c>
+      <c r="E3">
+        <v>30480618</v>
+      </c>
+      <c r="F3" s="37">
+        <f>Subsumes7!B13</f>
+        <v>171885898</v>
+      </c>
+      <c r="G3" s="37">
+        <f>Subsumes7!P13</f>
+        <v>28990053073.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f>C3/B3</f>
+        <v>1.2488093637288484</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:F5" si="0">D3/C3</f>
+        <v>0.99091857844362674</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1.530560808103653</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>5.6391867776434195</v>
+      </c>
+      <c r="G4">
+        <f>G3/F3</f>
+        <v>168.65870563447851</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.79349066977270277</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E6" si="1">E4/D4</f>
+        <v>1.544587861605752</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:G8" si="2">F4/E4</f>
+        <v>3.6843925101089621</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G6" si="3">G4/F4</f>
+        <v>29.90833825599228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>1.9465734386621114</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>2.3853563799722415</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>8.1175765540538922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1.2254129911541933</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>3.4030875311589108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>2.7770943802004311</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3419,7 +3597,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
     </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -3460,7 +3638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -3782,7 +3960,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
     </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -3823,7 +4001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -4341,7 +4519,7 @@
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
     </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -4382,7 +4560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -5116,7 +5294,7 @@
         <v>1.1491366080792502E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P21" s="8">
         <f>(I14-P14)/I14</f>
         <v>6.4429744790623529E-3</v>
@@ -5178,7 +5356,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5681,7 +5859,7 @@
       <c r="L19" s="33"/>
       <c r="M19" s="33"/>
     </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -5722,7 +5900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -5779,8 +5957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,10 +6043,12 @@
         <f>15^12</f>
         <v>129746337890625</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="13">
+        <v>161817578</v>
+      </c>
       <c r="C3" s="14">
         <f>B3/1000000000</f>
-        <v>0</v>
+        <v>0.16181757799999999</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -5877,14 +6057,16 @@
         <f>21^16</f>
         <v>1.4305686902419853E+21</v>
       </c>
-      <c r="P3" s="26"/>
+      <c r="P3" s="26">
+        <v>25303754288</v>
+      </c>
       <c r="Q3" s="14">
         <f>P3/1000000000</f>
-        <v>0</v>
+        <v>25.303754288</v>
       </c>
       <c r="R3" s="14">
         <f>Q3/60</f>
-        <v>0</v>
+        <v>0.42172923813333335</v>
       </c>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
@@ -5892,23 +6074,27 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="30"/>
-      <c r="B4" s="13"/>
+      <c r="B4" s="13">
+        <v>170859085</v>
+      </c>
       <c r="C4" s="14">
         <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
-        <v>0</v>
+        <v>0.17085908499999999</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="O4" s="30"/>
-      <c r="P4" s="26"/>
+      <c r="P4" s="26">
+        <v>30815589393</v>
+      </c>
       <c r="Q4" s="14">
         <f t="shared" ref="Q4:Q7" si="1">P4/1000000000</f>
-        <v>0</v>
+        <v>30.815589393</v>
       </c>
       <c r="R4" s="14">
         <f>Q4/60</f>
-        <v>0</v>
+        <v>0.51359315655000004</v>
       </c>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
@@ -5916,23 +6102,27 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="13">
+        <v>166944164</v>
+      </c>
       <c r="C5" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16694416400000001</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="O5" s="30"/>
-      <c r="P5" s="26"/>
+      <c r="P5" s="26">
+        <v>30869004997</v>
+      </c>
       <c r="Q5" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30.869004997000001</v>
       </c>
       <c r="R5" s="14">
         <f>Q5/60</f>
-        <v>0</v>
+        <v>0.51448341661666663</v>
       </c>
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
@@ -5940,147 +6130,196 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="13">
+        <v>170467072</v>
+      </c>
       <c r="C6" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.170467072</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="O6" s="30"/>
-      <c r="P6" s="26"/>
+      <c r="P6" s="26">
+        <v>30732405134</v>
+      </c>
       <c r="Q6" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="14"/>
+        <v>30.732405134</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" ref="R6:R11" si="2">Q6/60</f>
+        <v>0.51220675223333334</v>
+      </c>
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
       <c r="U6" s="15"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="30"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="13">
+        <v>173340649</v>
+      </c>
       <c r="C7" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.17334064900000001</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="O7" s="30"/>
-      <c r="P7" s="26"/>
+      <c r="P7" s="26">
+        <v>30745232266</v>
+      </c>
       <c r="Q7" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="14"/>
+        <v>30.745232265999999</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51242053776666663</v>
+      </c>
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="13">
+        <v>171589253</v>
+      </c>
       <c r="C8" s="14">
         <f>B8/1000000000</f>
-        <v>0</v>
+        <v>0.171589253</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="26"/>
+      <c r="P8" s="26">
+        <v>31324298061</v>
+      </c>
       <c r="Q8" s="14">
         <f>P8/1000000000</f>
-        <v>0</v>
-      </c>
-      <c r="R8" s="14"/>
+        <v>31.324298061</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="2"/>
+        <v>0.52207163435000004</v>
+      </c>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
       <c r="U8" s="15"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="13">
+        <v>173876630</v>
+      </c>
       <c r="C9" s="14">
         <f>B9/1000000000</f>
-        <v>0</v>
+        <v>0.17387663</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="O9" s="15"/>
-      <c r="P9" s="26"/>
+      <c r="P9" s="26">
+        <v>30733605439</v>
+      </c>
       <c r="Q9" s="14">
         <f>P9/1000000000</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="14"/>
+        <v>30.733605439000002</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51222675731666667</v>
+      </c>
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
       <c r="U9" s="15"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13">
+        <v>187445457</v>
+      </c>
       <c r="C10" s="14">
-        <f t="shared" ref="C10:C14" si="2">B10/1000000000</f>
-        <v>0</v>
+        <f t="shared" ref="C10:C14" si="3">B10/1000000000</f>
+        <v>0.18744545700000001</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="26"/>
+      <c r="P10" s="26">
+        <v>26954671901</v>
+      </c>
       <c r="Q10" s="14">
-        <f t="shared" ref="Q10:Q14" si="3">P10/1000000000</f>
-        <v>0</v>
-      </c>
-      <c r="R10" s="14"/>
+        <f t="shared" ref="Q10:Q14" si="4">P10/1000000000</f>
+        <v>26.954671901000001</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="2"/>
+        <v>0.44924453168333334</v>
+      </c>
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="13">
+        <v>174343839</v>
+      </c>
       <c r="C11" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.174343839</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="O11" s="15"/>
-      <c r="P11" s="26"/>
+      <c r="P11" s="26">
+        <v>25288023135</v>
+      </c>
       <c r="Q11" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="14"/>
+        <f t="shared" si="4"/>
+        <v>25.288023135</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" si="2"/>
+        <v>0.42146705224999997</v>
+      </c>
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
+      <c r="B12" s="18">
+        <v>168175253</v>
+      </c>
       <c r="C12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.168175253</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="O12" s="17"/>
-      <c r="P12" s="27"/>
+      <c r="P12" s="27">
+        <v>27133946121</v>
+      </c>
       <c r="Q12" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="21"/>
+        <f t="shared" si="4"/>
+        <v>27.133946121000001</v>
+      </c>
+      <c r="R12" s="19">
+        <f>Q12/60</f>
+        <v>0.45223243535000002</v>
+      </c>
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
       <c r="U12" s="15"/>
@@ -6089,13 +6328,13 @@
       <c r="A13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="20" t="e">
+      <c r="B13" s="20">
         <f>AVERAGE(B3:B12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13" s="21" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>171885898</v>
+      </c>
+      <c r="C13" s="21">
+        <f t="shared" si="3"/>
+        <v>0.17188589800000001</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -6105,21 +6344,21 @@
       <c r="O13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="20" t="e">
+      <c r="P13" s="20">
         <f>AVERAGE(P3:P12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q13" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R13" s="21" t="e">
+        <v>28990053073.5</v>
+      </c>
+      <c r="Q13" s="21">
+        <f t="shared" si="4"/>
+        <v>28.9900530735</v>
+      </c>
+      <c r="R13" s="21">
         <f>Q13/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" s="21" t="e">
+        <v>0.48316755122499999</v>
+      </c>
+      <c r="S13" s="21">
         <f>R13/60</f>
-        <v>#DIV/0!</v>
+        <v>8.0527925204166659E-3</v>
       </c>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
@@ -6128,13 +6367,13 @@
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="22" t="e">
+      <c r="B14" s="22">
         <f>B13/A3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C14" s="23" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.3247841965674459E-6</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" si="3"/>
+        <v>1.3247841965674459E-15</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -6142,21 +6381,21 @@
       <c r="O14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="P14" s="26" t="e">
+      <c r="P14" s="26">
         <f>P13/O3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q14" s="23" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R14" s="23" t="e">
+        <v>2.0264705407886594E-11</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" si="4"/>
+        <v>2.0264705407886594E-20</v>
+      </c>
+      <c r="R14" s="23">
         <f>Q14/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S14" s="15" t="e">
+        <v>3.3774509013144324E-22</v>
+      </c>
+      <c r="S14" s="15">
         <f>R14/60</f>
-        <v>#DIV/0!</v>
+        <v>5.6290848355240542E-24</v>
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
@@ -6184,25 +6423,25 @@
         <f>(55^33)</f>
         <v>2.703763826271497E+57</v>
       </c>
-      <c r="B17" s="13" t="e">
+      <c r="B17" s="13">
         <f>A17*$B$14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="13" t="e">
+        <v>3.5819035882952086E+51</v>
+      </c>
+      <c r="C17" s="13">
         <f>C14*A17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="15" t="e">
+        <v>3.5819035882952087E+42</v>
+      </c>
+      <c r="D17" s="15">
         <f>C17/(60*60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="15" t="e">
+        <v>9.9497321897089133E+38</v>
+      </c>
+      <c r="E17" s="15">
         <f>D17/24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="15" t="e">
+        <v>4.1457217457120472E+37</v>
+      </c>
+      <c r="F17" s="15">
         <f>E17/365</f>
-        <v>#DIV/0!</v>
+        <v>1.1358141769074102E+35</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -6225,7 +6464,7 @@
       <c r="O19" s="34"/>
       <c r="P19" s="34"/>
     </row>
-    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -6266,7 +6505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -6324,14 +6563,15 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.85546875" style="2"/>
     <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
     <col min="19" max="16384" width="10.85546875" style="2"/>
@@ -6792,9 +7032,13 @@
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2" t="e">
+      <c r="B11" s="3">
         <f>Subsumes7!B14</f>
-        <v>#DIV/0!</v>
+        <v>1.3247841965674459E-6</v>
+      </c>
+      <c r="C11" s="4">
+        <f>(B10-B11)/B10</f>
+        <v>-0.14214046453058282</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
@@ -6812,14 +7056,15 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.85546875" style="2"/>
     <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
     <col min="19" max="16384" width="10.85546875" style="2"/>
@@ -6887,7 +7132,7 @@
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="2">
         <f>Subsumes4!P14</f>
         <v>9.5419548041935121E-10</v>
       </c>
@@ -6972,9 +7217,13 @@
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="e">
+      <c r="B10" s="2">
         <f>Subsumes7!P14</f>
-        <v>#DIV/0!</v>
+        <v>2.0264705407886594E-11</v>
+      </c>
+      <c r="C10" s="4">
+        <f>(B9-B10)/B9</f>
+        <v>-0.1535071446640279</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Time test subsumes 7
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
     <sheet name="Grafiek7" sheetId="13" r:id="rId11"/>
     <sheet name="Sheet1" sheetId="15" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="33">
   <si>
     <t>Tester</t>
   </si>
@@ -197,25 +202,10 @@
     <t>Subsumes + Redundant Comparators + Permutation optilmalisation + Lemma 4 + test array/hash/… + Lemma 5 + Lemma 6</t>
   </si>
   <si>
-    <t>2 kanalen</t>
+    <t>Subsumes7</t>
   </si>
   <si>
-    <t>3 kanalen</t>
-  </si>
-  <si>
-    <t>4 kanalen</t>
-  </si>
-  <si>
-    <t>5 kanalen</t>
-  </si>
-  <si>
-    <t>6 kanalen</t>
-  </si>
-  <si>
-    <t>7 kanalen</t>
-  </si>
-  <si>
-    <t>Subsumes7</t>
+    <t>kanalen</t>
   </si>
 </sst>
 </file>
@@ -223,13 +213,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="169" formatCode="0.0000%"/>
-    <numFmt numFmtId="170" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0000%"/>
+    <numFmt numFmtId="169" formatCode="0.0000000E+00"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -380,7 +370,7 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -388,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,7 +387,7 @@
     <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -409,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -420,16 +410,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -437,10 +427,10 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -448,7 +438,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -459,19 +453,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -498,7 +488,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -524,7 +513,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -590,7 +579,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-BE"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -603,7 +592,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -660,25 +648,25 @@
                 <c:formatCode>_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.5123353774301645E-4</c:v>
+                  <c:v>0.000151233537743016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1208736842005942E-4</c:v>
+                  <c:v>0.000112087368420059</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0581533388767822E-4</c:v>
+                  <c:v>0.000105815333887678</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5749834390105394E-5</c:v>
+                  <c:v>1.57498343901054E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5487632479415025E-5</c:v>
+                  <c:v>1.5487632479415E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1599135462834068E-6</c:v>
+                  <c:v>1.15991354628341E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3247841965674459E-6</c:v>
+                  <c:v>1.32478419656745E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,11 +682,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="75999872"/>
-        <c:axId val="78779904"/>
+        <c:axId val="-2093744016"/>
+        <c:axId val="2116959552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75999872"/>
+        <c:axId val="-2093744016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,10 +726,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78779904"/>
+        <c:crossAx val="2116959552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -749,7 +737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78779904"/>
+        <c:axId val="2116959552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,10 +797,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75999872"/>
+        <c:crossAx val="-2093744016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -866,7 +854,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -887,7 +875,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -913,7 +900,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -979,7 +966,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-BE"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -992,7 +979,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1037,13 +1023,13 @@
                 <c:formatCode>0.0000000E+00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>9.5419548041935121E-10</c:v>
+                  <c:v>9.54195480419351E-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7567906277502009E-11</c:v>
+                  <c:v>1.7567906277502E-11</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>2.0264705407886594E-11</c:v>
+                  <c:v>2.02647054078866E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,11 +1045,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="84308736"/>
-        <c:axId val="84311424"/>
+        <c:axId val="-2093820032"/>
+        <c:axId val="-2093823552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84308736"/>
+        <c:axId val="-2093820032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,10 +1089,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84311424"/>
+        <c:crossAx val="-2093823552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1114,7 +1100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84311424"/>
+        <c:axId val="-2093823552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,10 +1160,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84308736"/>
+        <c:crossAx val="-2093820032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1231,9 +1217,456 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-BE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[ns]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$I$3</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[s]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="nl-NL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.016093076</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.020097184</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.019914673</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.030480618</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.171885898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.9900530735</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>201.760599999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2090252160"/>
+        <c:axId val="-2090299312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2090252160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2090299312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2090299312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2090252160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1317,6 +1750,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
@@ -2453,6 +2926,509 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2530,6 +3506,41 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2791</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6978</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>122535</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2826,14 +3837,14 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2857,14 +3868,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -3040,14 +4051,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -3076,16 +4087,16 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -3126,7 +4137,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -3179,150 +4190,199 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3">
         <v>16093076</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>20097184</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>19914673</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>30480618</v>
       </c>
-      <c r="F3" s="37">
+      <c r="G3" s="33">
         <f>Subsumes7!B13</f>
         <v>171885898</v>
       </c>
-      <c r="G3" s="37">
+      <c r="H3" s="33">
         <f>Subsumes7!P13</f>
         <v>28990053073.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="32">
+        <v>0</v>
+      </c>
       <c r="C4">
-        <f>C3/B3</f>
-        <v>1.2488093637288484</v>
+        <f>C3/(10^9)</f>
+        <v>1.6093076000000001E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:F5" si="0">D3/C3</f>
-        <v>0.99091857844362674</v>
+        <f t="shared" ref="D4:H4" si="0">D3/(10^9)</f>
+        <v>2.0097184000000001E-2</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1.530560808103653</v>
+        <v>1.9914673000000001E-2</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
+        <v>3.0480618000000001E-2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.17188589800000001</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>28.9900530735</v>
+      </c>
+      <c r="I4">
+        <f>0.0392*I2^6 -0.8223*I2^5+6.8477*I2^4 - 28.743*I2^3 + 63.47*I2^2 - 68.887*I2 + 28.095</f>
+        <v>201.76059999999799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f>D3/C3</f>
+        <v>1.2488093637288484</v>
+      </c>
+      <c r="E5">
+        <f>E3/D3</f>
+        <v>0.99091857844362674</v>
+      </c>
+      <c r="F5">
+        <f>F3/E3</f>
+        <v>1.530560808103653</v>
+      </c>
+      <c r="G5">
+        <f>G3/F3</f>
         <v>5.6391867776434195</v>
       </c>
-      <c r="G4">
-        <f>G3/F3</f>
+      <c r="H5">
+        <f>H3/G3</f>
         <v>168.65870563447851</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <f t="shared" si="0"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <f t="shared" ref="E6" si="1">E5/D5</f>
         <v>0.79349066977270277</v>
       </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E6" si="1">E4/D4</f>
+      <c r="F6">
+        <f t="shared" ref="F6:F7" si="2">F5/E5</f>
         <v>1.544587861605752</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:G8" si="2">F4/E4</f>
+      <c r="G6">
+        <f t="shared" ref="G6:H9" si="3">G5/F5</f>
         <v>3.6843925101089621</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G6" si="3">G4/F4</f>
+      <c r="H6">
+        <f t="shared" ref="H6:H7" si="4">H5/G5</f>
         <v>29.90833825599228</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>1.9465734386621114</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>2.3853563799722415</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
-        <v>8.1175765540538922</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F7">
         <f t="shared" si="2"/>
+        <v>1.9465734386621114</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>2.3853563799722415</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>8.1175765540538922</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f t="shared" si="3"/>
         <v>1.2254129911541933</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
+      <c r="H8">
+        <f t="shared" si="3"/>
         <v>3.4030875311589108</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8">
-        <f t="shared" si="2"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <f t="shared" si="3"/>
         <v>2.7770943802004311</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3334,16 +4394,16 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -3367,14 +4427,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -3552,14 +4612,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -3588,16 +4648,16 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -3638,7 +4698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -3698,15 +4758,15 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -3730,14 +4790,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -3915,14 +4975,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -3951,16 +5011,16 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -4001,7 +5061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -4061,20 +5121,20 @@
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -4119,24 +5179,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -4474,14 +5534,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -4510,16 +5570,16 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -4560,7 +5620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -4621,17 +5681,17 @@
       <selection activeCell="A22" sqref="A22:T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="28" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" style="28" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -4691,30 +5751,30 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="H2" s="32" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="O2" s="32" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="O2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -5185,30 +6245,30 @@
       <c r="T15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="H16" s="32" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="H16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="O16" s="32" t="s">
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="O16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -5294,35 +6354,35 @@
         <v>1.1491366080792502E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P21" s="8">
         <f>(I14-P14)/I14</f>
         <v>6.4429744790623529E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5334,7 +6394,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="I14 B14 P14">
+  <conditionalFormatting sqref="B14 I14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5359,20 +6419,20 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -5417,24 +6477,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -5807,14 +6867,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -5842,24 +6902,24 @@
         <v>9.9446102487422776E+34</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -5900,7 +6960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -5961,20 +7021,20 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -6019,24 +7079,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -6409,14 +7469,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -6444,27 +7504,27 @@
         <v>1.1358141769074102E+35</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-    </row>
-    <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+    </row>
+    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -6505,7 +7565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -6566,23 +7626,23 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" style="2"/>
-    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="18" width="7.83203125" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -6642,7 +7702,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -6707,7 +7767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G4" s="7">
         <f>ABS(G2-G3)/G2</f>
         <v>0</v>
@@ -6757,7 +7817,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -6825,7 +7885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G6" s="7">
         <f>ABS(G3-G5)/G3</f>
         <v>0</v>
@@ -6875,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -6943,7 +8003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G8" s="7">
         <f>ABS(G5-G7)/G5</f>
         <v>0</v>
@@ -6993,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -7011,7 +8071,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -7028,7 +8088,7 @@
         <v>0.99233031532824156</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -7041,7 +8101,7 @@
         <v>-0.14214046453058282</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -7059,30 +8119,30 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" style="2"/>
-    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="18" width="7.83203125" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="3"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -7091,7 +8151,7 @@
       <c r="D3" s="4"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -7105,7 +8165,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -7114,7 +8174,7 @@
       <c r="D5" s="4"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -7128,7 +8188,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -7190,7 +8250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -7199,7 +8259,7 @@
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -7213,7 +8273,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -7226,7 +8286,7 @@
         <v>-0.1535071446640279</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Kleine update aan de tijdsvoorstelling grafieken
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -488,6 +488,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -592,6 +593,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -682,11 +684,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2093744016"/>
-        <c:axId val="2116959552"/>
+        <c:axId val="-2056991536"/>
+        <c:axId val="-2063258432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093744016"/>
+        <c:axId val="-2056991536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,7 +731,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2116959552"/>
+        <c:crossAx val="-2063258432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -737,9 +739,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116959552"/>
+        <c:axId val="-2063258432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.000155"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -800,9 +804,10 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093744016"/>
+        <c:crossAx val="-2056991536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0E-5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -875,6 +880,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -979,6 +985,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1045,11 +1052,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2093820032"/>
-        <c:axId val="-2093823552"/>
+        <c:axId val="-2063530704"/>
+        <c:axId val="-2089696480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093820032"/>
+        <c:axId val="-2063530704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1099,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093823552"/>
+        <c:crossAx val="-2089696480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1100,9 +1107,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093823552"/>
+        <c:axId val="-2089696480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0E-9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1163,9 +1171,10 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093820032"/>
+        <c:crossAx val="-2063530704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0E-10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1514,11 +1523,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2090252160"/>
-        <c:axId val="-2090299312"/>
+        <c:axId val="-2092931344"/>
+        <c:axId val="-2128154560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2090252160"/>
+        <c:axId val="-2092931344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1570,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090299312"/>
+        <c:crossAx val="-2128154560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1569,7 +1578,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090299312"/>
+        <c:axId val="-2128154560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1621,7 +1630,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090252160"/>
+        <c:crossAx val="-2092931344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3437,7 +3446,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3448,7 +3457,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3459,7 +3468,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6079191"/>
+    <xdr:ext cx="9313333" cy="6079537"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -3486,7 +3495,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6079191"/>
+    <xdr:ext cx="9313333" cy="6079537"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -4192,7 +4201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+    <sheetView zoomScale="182" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -6394,7 +6403,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14 I14 P14">
+  <conditionalFormatting sqref="I14 B14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Performed a re-test on Subsumes7.
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -25,7 +20,7 @@
     <sheet name="Grafiek7" sheetId="13" r:id="rId11"/>
     <sheet name="Sheet1" sheetId="15" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -213,13 +208,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="168" formatCode="0.0000%"/>
-    <numFmt numFmtId="169" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.0000%"/>
+    <numFmt numFmtId="170" formatCode="0.0000000E+00"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -370,7 +365,7 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -378,7 +373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,7 +382,7 @@
     <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -410,16 +405,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -427,10 +422,10 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -438,7 +433,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -457,11 +452,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Komma" xfId="2" builtinId="3"/>
-    <cellStyle name="Procent" xfId="1" builtinId="5"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -514,7 +509,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -580,7 +575,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="nl-BE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -650,25 +645,25 @@
                 <c:formatCode>_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.000151233537743016</c:v>
+                  <c:v>1.5123353774301645E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000112087368420059</c:v>
+                  <c:v>1.1208736842005942E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000105815333887678</c:v>
+                  <c:v>1.0581533388767822E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.57498343901054E-5</c:v>
+                  <c:v>1.5749834390105394E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5487632479415E-5</c:v>
+                  <c:v>1.5487632479415025E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.15991354628341E-6</c:v>
+                  <c:v>1.1599135462834068E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.32478419656745E-6</c:v>
+                  <c:v>1.3247841965674459E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -684,11 +679,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2056991536"/>
-        <c:axId val="-2063258432"/>
+        <c:axId val="61784064"/>
+        <c:axId val="61786752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2056991536"/>
+        <c:axId val="61784064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,10 +723,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063258432"/>
+        <c:crossAx val="61786752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -739,11 +734,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2063258432"/>
+        <c:axId val="61786752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.000155"/>
-          <c:min val="0.0"/>
+          <c:max val="1.55E-4"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -801,13 +796,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056991536"/>
+        <c:crossAx val="61784064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0E-5"/>
+        <c:majorUnit val="1.0000000000000001E-5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -859,7 +854,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -880,7 +875,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -906,7 +900,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -972,7 +966,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="nl-BE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -1030,13 +1024,13 @@
                 <c:formatCode>0.0000000E+00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>9.54195480419351E-10</c:v>
+                  <c:v>9.5419548041935121E-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7567906277502E-11</c:v>
+                  <c:v>1.7567906277502009E-11</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>2.02647054078866E-11</c:v>
+                  <c:v>1.9377505144133226E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1052,11 +1046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2063530704"/>
-        <c:axId val="-2089696480"/>
+        <c:axId val="68945792"/>
+        <c:axId val="68948736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2063530704"/>
+        <c:axId val="68945792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,10 +1090,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089696480"/>
+        <c:crossAx val="68948736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1107,10 +1101,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2089696480"/>
+        <c:axId val="68948736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0E-9"/>
+          <c:max val="1.0000000000000001E-9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1168,13 +1162,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063530704"/>
+        <c:crossAx val="68945792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0E-10"/>
+        <c:majorUnit val="1E-10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1226,7 +1220,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1247,7 +1241,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1273,7 +1266,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1328,28 +1321,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,7 +1407,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1440,7 +1432,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="nl-NL"/>
+                  <a:endParaRPr lang="nl-BE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1452,28 +1444,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1485,28 +1477,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.016093076</c:v>
+                  <c:v>1.6093076000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.020097184</c:v>
+                  <c:v>2.0097184000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.019914673</c:v>
+                  <c:v>1.9914673000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.030480618</c:v>
+                  <c:v>3.0480618000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.171885898</c:v>
+                  <c:v>0.17188589800000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.9900530735</c:v>
+                  <c:v>27.720852154199999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>201.760599999998</c:v>
+                  <c:v>201.76059999999799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1523,11 +1515,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2092931344"/>
-        <c:axId val="-2128154560"/>
+        <c:axId val="69003520"/>
+        <c:axId val="69087232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2092931344"/>
+        <c:axId val="69003520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,10 +1559,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128154560"/>
+        <c:crossAx val="69087232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1578,10 +1570,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128154560"/>
+        <c:axId val="69087232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.0"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1627,10 +1619,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092931344"/>
+        <c:crossAx val="69003520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1668,7 +1660,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3446,7 +3438,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3468,7 +3460,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6079537"/>
+    <xdr:ext cx="9300882" cy="6079191"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -3846,14 +3838,14 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -4205,12 +4197,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -4277,7 +4269,7 @@
       </c>
       <c r="H3" s="33">
         <f>Subsumes7!P13</f>
-        <v>28990053073.5</v>
+        <v>27720852154.200001</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4309,7 +4301,7 @@
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>28.9900530735</v>
+        <v>27.720852154199999</v>
       </c>
       <c r="I4">
         <f>0.0392*I2^6 -0.8223*I2^5+6.8477*I2^4 - 28.743*I2^3 + 63.47*I2^2 - 68.887*I2 + 28.095</f>
@@ -4335,7 +4327,7 @@
       </c>
       <c r="H5">
         <f>H3/G3</f>
-        <v>168.65870563447851</v>
+        <v>161.27473211444024</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4353,7 +4345,7 @@
       </c>
       <c r="H6">
         <f t="shared" ref="H6:H7" si="4">H5/G5</f>
-        <v>29.90833825599228</v>
+        <v>28.598934292053354</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4367,7 +4359,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="4"/>
-        <v>8.1175765540538922</v>
+        <v>7.7621844615050444</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -4377,13 +4369,13 @@
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>3.4030875311589108</v>
+        <v>3.2540984343795931</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>2.7770943802004311</v>
+        <v>2.6555116176095206</v>
       </c>
     </row>
   </sheetData>
@@ -4403,16 +4395,16 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -4767,15 +4759,15 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -5130,20 +5122,20 @@
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" style="11"/>
-    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="11"/>
+    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -5690,17 +5682,17 @@
       <selection activeCell="A22" sqref="A22:T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.83203125" style="28" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" style="28" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -6369,7 +6361,7 @@
         <v>6.4429744790623529E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>28</v>
       </c>
@@ -6403,7 +6395,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="I14 B14 P14">
+  <conditionalFormatting sqref="B14 I14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6428,20 +6420,20 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" style="11"/>
-    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="11"/>
+    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -6911,7 +6903,7 @@
         <v>9.9446102487422776E+34</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>29</v>
       </c>
@@ -7027,23 +7019,23 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" style="11"/>
-    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="11"/>
+    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -7127,15 +7119,15 @@
         <v>1.4305686902419853E+21</v>
       </c>
       <c r="P3" s="26">
-        <v>25303754288</v>
+        <v>24823921974</v>
       </c>
       <c r="Q3" s="14">
         <f>P3/1000000000</f>
-        <v>25.303754288</v>
+        <v>24.823921974000001</v>
       </c>
       <c r="R3" s="14">
         <f>Q3/60</f>
-        <v>0.42172923813333335</v>
+        <v>0.41373203289999999</v>
       </c>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
@@ -7155,15 +7147,15 @@
       <c r="F4" s="15"/>
       <c r="O4" s="30"/>
       <c r="P4" s="26">
-        <v>30815589393</v>
+        <v>29165320450</v>
       </c>
       <c r="Q4" s="14">
         <f t="shared" ref="Q4:Q7" si="1">P4/1000000000</f>
-        <v>30.815589393</v>
+        <v>29.165320449999999</v>
       </c>
       <c r="R4" s="14">
         <f>Q4/60</f>
-        <v>0.51359315655000004</v>
+        <v>0.48608867416666668</v>
       </c>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
@@ -7183,15 +7175,15 @@
       <c r="F5" s="15"/>
       <c r="O5" s="30"/>
       <c r="P5" s="26">
-        <v>30869004997</v>
+        <v>24624222015</v>
       </c>
       <c r="Q5" s="14">
         <f t="shared" si="1"/>
-        <v>30.869004997000001</v>
+        <v>24.624222015000001</v>
       </c>
       <c r="R5" s="14">
         <f>Q5/60</f>
-        <v>0.51448341661666663</v>
+        <v>0.41040370025</v>
       </c>
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
@@ -7211,15 +7203,15 @@
       <c r="F6" s="15"/>
       <c r="O6" s="30"/>
       <c r="P6" s="26">
-        <v>30732405134</v>
+        <v>28927545003</v>
       </c>
       <c r="Q6" s="14">
         <f t="shared" si="1"/>
-        <v>30.732405134</v>
+        <v>28.927545002999999</v>
       </c>
       <c r="R6" s="14">
         <f t="shared" ref="R6:R11" si="2">Q6/60</f>
-        <v>0.51220675223333334</v>
+        <v>0.48212575004999997</v>
       </c>
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
@@ -7239,15 +7231,15 @@
       <c r="F7" s="15"/>
       <c r="O7" s="30"/>
       <c r="P7" s="26">
-        <v>30745232266</v>
+        <v>24258287724</v>
       </c>
       <c r="Q7" s="14">
         <f t="shared" si="1"/>
-        <v>30.745232265999999</v>
+        <v>24.258287723999999</v>
       </c>
       <c r="R7" s="14">
         <f t="shared" si="2"/>
-        <v>0.51242053776666663</v>
+        <v>0.40430479539999997</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
@@ -7267,15 +7259,15 @@
       <c r="F8" s="15"/>
       <c r="O8" s="15"/>
       <c r="P8" s="26">
-        <v>31324298061</v>
+        <v>29171312688</v>
       </c>
       <c r="Q8" s="14">
         <f>P8/1000000000</f>
-        <v>31.324298061</v>
+        <v>29.171312688</v>
       </c>
       <c r="R8" s="14">
         <f t="shared" si="2"/>
-        <v>0.52207163435000004</v>
+        <v>0.48618854480000001</v>
       </c>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
@@ -7295,15 +7287,15 @@
       <c r="F9" s="15"/>
       <c r="O9" s="15"/>
       <c r="P9" s="26">
-        <v>30733605439</v>
+        <v>29036512816</v>
       </c>
       <c r="Q9" s="14">
         <f>P9/1000000000</f>
-        <v>30.733605439000002</v>
+        <v>29.036512815999998</v>
       </c>
       <c r="R9" s="14">
         <f t="shared" si="2"/>
-        <v>0.51222675731666667</v>
+        <v>0.48394188026666662</v>
       </c>
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
@@ -7323,15 +7315,15 @@
       <c r="F10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="26">
-        <v>26954671901</v>
+        <v>29133569029</v>
       </c>
       <c r="Q10" s="14">
         <f t="shared" ref="Q10:Q14" si="4">P10/1000000000</f>
-        <v>26.954671901000001</v>
+        <v>29.133569029</v>
       </c>
       <c r="R10" s="14">
         <f t="shared" si="2"/>
-        <v>0.44924453168333334</v>
+        <v>0.48555948381666669</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
@@ -7351,15 +7343,15 @@
       <c r="F11" s="15"/>
       <c r="O11" s="15"/>
       <c r="P11" s="26">
-        <v>25288023135</v>
+        <v>29088751267</v>
       </c>
       <c r="Q11" s="14">
         <f t="shared" si="4"/>
-        <v>25.288023135</v>
+        <v>29.088751266999999</v>
       </c>
       <c r="R11" s="14">
         <f t="shared" si="2"/>
-        <v>0.42146705224999997</v>
+        <v>0.48481252111666667</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
@@ -7379,15 +7371,15 @@
       <c r="F12" s="15"/>
       <c r="O12" s="17"/>
       <c r="P12" s="27">
-        <v>27133946121</v>
+        <v>28979078576</v>
       </c>
       <c r="Q12" s="19">
         <f t="shared" si="4"/>
-        <v>27.133946121000001</v>
+        <v>28.979078575999999</v>
       </c>
       <c r="R12" s="19">
         <f>Q12/60</f>
-        <v>0.45223243535000002</v>
+        <v>0.48298464293333332</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
@@ -7415,19 +7407,19 @@
       </c>
       <c r="P13" s="20">
         <f>AVERAGE(P3:P12)</f>
-        <v>28990053073.5</v>
+        <v>27720852154.200001</v>
       </c>
       <c r="Q13" s="21">
         <f t="shared" si="4"/>
-        <v>28.9900530735</v>
+        <v>27.720852154199999</v>
       </c>
       <c r="R13" s="21">
         <f>Q13/60</f>
-        <v>0.48316755122499999</v>
+        <v>0.46201420256999998</v>
       </c>
       <c r="S13" s="21">
         <f>R13/60</f>
-        <v>8.0527925204166659E-3</v>
+        <v>7.7002367094999996E-3</v>
       </c>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
@@ -7452,19 +7444,19 @@
       </c>
       <c r="P14" s="26">
         <f>P13/O3</f>
-        <v>2.0264705407886594E-11</v>
+        <v>1.9377505144133226E-11</v>
       </c>
       <c r="Q14" s="23">
         <f t="shared" si="4"/>
-        <v>2.0264705407886594E-20</v>
+        <v>1.9377505144133225E-20</v>
       </c>
       <c r="R14" s="23">
         <f>Q14/60</f>
-        <v>3.3774509013144324E-22</v>
+        <v>3.229584190688871E-22</v>
       </c>
       <c r="S14" s="15">
         <f>R14/60</f>
-        <v>5.6290848355240542E-24</v>
+        <v>5.382640317814785E-24</v>
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
@@ -7513,7 +7505,7 @@
         <v>1.1358141769074102E+35</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>30</v>
       </c>
@@ -7635,23 +7627,23 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="18" width="7.83203125" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" style="2"/>
+    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -7711,7 +7703,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -7776,7 +7768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
       <c r="G4" s="7">
         <f>ABS(G2-G3)/G2</f>
         <v>0</v>
@@ -7826,7 +7818,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -7894,7 +7886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
       <c r="G6" s="7">
         <f>ABS(G3-G5)/G3</f>
         <v>0</v>
@@ -7944,7 +7936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -8012,7 +8004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
       <c r="G8" s="7">
         <f>ABS(G5-G7)/G5</f>
         <v>0</v>
@@ -8062,7 +8054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -8080,7 +8072,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -8097,7 +8089,7 @@
         <v>0.99233031532824156</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -8110,7 +8102,7 @@
         <v>-0.14214046453058282</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -8124,34 +8116,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="18" width="7.83203125" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" style="2"/>
+    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="3"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -8160,7 +8152,7 @@
       <c r="D3" s="4"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -8174,7 +8166,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -8183,7 +8175,7 @@
       <c r="D5" s="4"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -8197,7 +8189,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -8259,7 +8251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -8268,7 +8260,7 @@
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -8282,20 +8274,20 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2">
         <f>Subsumes7!P14</f>
-        <v>2.0264705407886594E-11</v>
+        <v>1.9377505144133226E-11</v>
       </c>
       <c r="C10" s="4">
         <f>(B9-B10)/B9</f>
-        <v>-0.1535071446640279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+        <v>-0.10300594948805275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Added time tests for subsumes9.
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,11 @@
     <sheet name="Subsumes6" sheetId="11" r:id="rId6"/>
     <sheet name="Subsumes7" sheetId="14" r:id="rId7"/>
     <sheet name="Subsumes8" sheetId="16" r:id="rId8"/>
-    <sheet name="Samenvatting_6" sheetId="6" r:id="rId9"/>
-    <sheet name="Samenvatting_7" sheetId="12" r:id="rId10"/>
-    <sheet name="Grafiek6" sheetId="8" r:id="rId11"/>
-    <sheet name="Grafiek7" sheetId="13" r:id="rId12"/>
+    <sheet name="Subsumes9" sheetId="17" r:id="rId9"/>
+    <sheet name="Samenvatting_6" sheetId="6" r:id="rId10"/>
+    <sheet name="Samenvatting_7" sheetId="12" r:id="rId11"/>
+    <sheet name="Grafiek6" sheetId="8" r:id="rId12"/>
+    <sheet name="Grafiek7" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="34">
   <si>
     <t>Tester</t>
   </si>
@@ -199,6 +200,12 @@
   <si>
     <t>Subsumes + Redundant Comparators + Permutation optilmalisation + Lemma 4 + test array/hash/… + Lemma 5 + Lemma 6 + Unique_2</t>
   </si>
+  <si>
+    <t>Subsumes + Redundant Comparators + Permutation optilmalisation + Lemma 4 + test array/hash/… + Lemma 5 + Lemma 6 + Unique_2 + LookupTable</t>
+  </si>
+  <si>
+    <t>Subsumes 9</t>
+  </si>
 </sst>
 </file>
 
@@ -366,7 +373,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -437,6 +444,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -476,6 +486,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -674,11 +685,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="44122880"/>
-        <c:axId val="44124416"/>
+        <c:axId val="44946176"/>
+        <c:axId val="44947712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44122880"/>
+        <c:axId val="44946176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -721,7 +732,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44124416"/>
+        <c:crossAx val="44947712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -729,7 +740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44124416"/>
+        <c:axId val="44947712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.55E-4"/>
@@ -794,7 +805,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44122880"/>
+        <c:crossAx val="44946176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0000000000000001E-5"/>
@@ -870,7 +881,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1029,7 +1039,7 @@
                   <c:v>1.9377505144133226E-11</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1.2648026325977652E-11</c:v>
+                  <c:v>1.0273223719732067E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1045,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="44471424"/>
-        <c:axId val="44478464"/>
+        <c:axId val="44807296"/>
+        <c:axId val="44810240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44471424"/>
+        <c:axId val="44807296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1102,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44478464"/>
+        <c:crossAx val="44810240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1100,7 +1110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44478464"/>
+        <c:axId val="44810240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0000000000000001E-9"/>
@@ -1164,7 +1174,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44471424"/>
+        <c:crossAx val="44807296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1E-10"/>
@@ -2845,14 +2855,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -3028,14 +3038,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -3064,14 +3074,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -3167,10 +3177,637 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" style="2"/>
+    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3">
+        <f>Subsumes1!B14</f>
+        <v>1.5123353774301645E-4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5">
+        <f>Subsumes1!B22</f>
+        <v>15</v>
+      </c>
+      <c r="H2" s="5">
+        <f>Subsumes1!C22</f>
+        <v>15</v>
+      </c>
+      <c r="I2" s="5">
+        <f>Subsumes1!D22</f>
+        <v>45</v>
+      </c>
+      <c r="J2" s="5">
+        <f>Subsumes1!E22</f>
+        <v>105</v>
+      </c>
+      <c r="K2" s="5">
+        <f>Subsumes1!F22</f>
+        <v>255</v>
+      </c>
+      <c r="L2" s="5">
+        <f>Subsumes1!G22</f>
+        <v>540</v>
+      </c>
+      <c r="M2" s="5">
+        <f>Subsumes1!H22</f>
+        <v>795</v>
+      </c>
+      <c r="N2" s="5">
+        <f>Subsumes1!I22</f>
+        <v>795</v>
+      </c>
+      <c r="O2" s="5">
+        <f>Subsumes1!J22</f>
+        <v>660</v>
+      </c>
+      <c r="P2" s="5">
+        <f>Subsumes1!K22</f>
+        <v>345</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>Subsumes1!L22</f>
+        <v>120</v>
+      </c>
+      <c r="R2" s="5">
+        <f>Subsumes1!M22</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3">
+        <f>Subsumes2!B14</f>
+        <v>1.1208736842005942E-4</v>
+      </c>
+      <c r="C3" s="4">
+        <f>(B2-B3)/B2</f>
+        <v>0.25884582154968927</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5">
+        <f>Subsumes2!B22</f>
+        <v>15</v>
+      </c>
+      <c r="H3" s="5">
+        <f>Subsumes2!C22</f>
+        <v>14</v>
+      </c>
+      <c r="I3" s="5">
+        <f>Subsumes2!D22</f>
+        <v>39</v>
+      </c>
+      <c r="J3" s="5">
+        <f>Subsumes2!E22</f>
+        <v>84</v>
+      </c>
+      <c r="K3" s="5">
+        <f>Subsumes2!F22</f>
+        <v>186</v>
+      </c>
+      <c r="L3" s="5">
+        <f>Subsumes2!G22</f>
+        <v>355</v>
+      </c>
+      <c r="M3" s="5">
+        <f>Subsumes2!H22</f>
+        <v>457</v>
+      </c>
+      <c r="N3" s="5">
+        <f>Subsumes2!I22</f>
+        <v>382</v>
+      </c>
+      <c r="O3" s="5">
+        <f>Subsumes2!J22</f>
+        <v>257</v>
+      </c>
+      <c r="P3" s="5">
+        <f>Subsumes2!K22</f>
+        <v>100</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>Subsumes2!L22</f>
+        <v>21</v>
+      </c>
+      <c r="R3" s="5">
+        <f>Subsumes2!M22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+      <c r="G4" s="7">
+        <f>ABS(G2-G3)/G2</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" ref="H4:R4" si="0">ABS(H2-H3)/H2</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.27058823529411763</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.34259259259259262</v>
+      </c>
+      <c r="M4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.42515723270440253</v>
+      </c>
+      <c r="N4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.51949685534591195</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.6106060606060606</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.71014492753623193</v>
+      </c>
+      <c r="Q4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3">
+        <f>Subsumes3!B14</f>
+        <v>1.0581533388767822E-4</v>
+      </c>
+      <c r="C5" s="4">
+        <f>(B3-B5)/B3</f>
+        <v>5.5956657924879416E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <f>ABS(B2-B5)/B2</f>
+        <v>0.30031833238282835</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5">
+        <f>Subsumes3!B22</f>
+        <v>15</v>
+      </c>
+      <c r="H5" s="5">
+        <f>Subsumes3!C22</f>
+        <v>14</v>
+      </c>
+      <c r="I5" s="5">
+        <f>Subsumes3!D22</f>
+        <v>39</v>
+      </c>
+      <c r="J5" s="5">
+        <f>Subsumes3!E22</f>
+        <v>84</v>
+      </c>
+      <c r="K5" s="5">
+        <f>Subsumes3!F22</f>
+        <v>186</v>
+      </c>
+      <c r="L5" s="5">
+        <f>Subsumes3!G22</f>
+        <v>355</v>
+      </c>
+      <c r="M5" s="5">
+        <f>Subsumes3!H22</f>
+        <v>457</v>
+      </c>
+      <c r="N5" s="5">
+        <f>Subsumes3!I22</f>
+        <v>382</v>
+      </c>
+      <c r="O5" s="5">
+        <f>Subsumes3!J22</f>
+        <v>257</v>
+      </c>
+      <c r="P5" s="5">
+        <f>Subsumes3!K22</f>
+        <v>100</v>
+      </c>
+      <c r="Q5" s="5">
+        <f>Subsumes3!L22</f>
+        <v>21</v>
+      </c>
+      <c r="R5" s="5">
+        <f>Subsumes3!M22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+      <c r="G6" s="7">
+        <f>ABS(G3-G5)/G3</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" ref="H6:R6" si="1">ABS(H3-H5)/H3</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3">
+        <f>Subsumes4!B14</f>
+        <v>1.5749834390105394E-5</v>
+      </c>
+      <c r="C7" s="4">
+        <f>(B5-B7)/B5</f>
+        <v>0.85115735298984496</v>
+      </c>
+      <c r="D7" s="4">
+        <f>(B2-B7)/B2</f>
+        <v>0.89585752852738065</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5">
+        <f>Subsumes4!B22</f>
+        <v>15</v>
+      </c>
+      <c r="H7" s="5">
+        <f>Subsumes4!C22</f>
+        <v>14</v>
+      </c>
+      <c r="I7" s="5">
+        <f>Subsumes4!D22</f>
+        <v>39</v>
+      </c>
+      <c r="J7" s="5">
+        <f>Subsumes4!E22</f>
+        <v>84</v>
+      </c>
+      <c r="K7" s="5">
+        <f>Subsumes4!F22</f>
+        <v>186</v>
+      </c>
+      <c r="L7" s="5">
+        <f>Subsumes4!G22</f>
+        <v>355</v>
+      </c>
+      <c r="M7" s="5">
+        <f>Subsumes4!H22</f>
+        <v>457</v>
+      </c>
+      <c r="N7" s="5">
+        <f>Subsumes4!I22</f>
+        <v>382</v>
+      </c>
+      <c r="O7" s="5">
+        <f>Subsumes4!J22</f>
+        <v>257</v>
+      </c>
+      <c r="P7" s="5">
+        <f>Subsumes4!K22</f>
+        <v>100</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>Subsumes4!L22</f>
+        <v>21</v>
+      </c>
+      <c r="R7" s="5">
+        <f>Subsumes4!M22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+      <c r="G8" s="7">
+        <f>ABS(G5-G7)/G5</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" ref="H8:R8" si="2">ABS(H5-H7)/H5</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <f>MIN(Subsumes5!B14,Subsumes5!I14,Subsumes5!P14)</f>
+        <v>1.5487632479415025E-5</v>
+      </c>
+      <c r="C9" s="4">
+        <f>(B7-B9)/B7</f>
+        <v>1.6647915412691134E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <f>(B2-B9)/B2</f>
+        <v>0.89759128358332552</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3">
+        <f>Subsumes6!B14</f>
+        <v>1.1599135462834068E-6</v>
+      </c>
+      <c r="C10" s="4">
+        <f>(B9-B10)/B9</f>
+        <v>0.92510711060421436</v>
+      </c>
+      <c r="D10" s="4">
+        <f>(B2-B10)/B2</f>
+        <v>0.99233031532824156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3">
+        <f>Subsumes7!B14</f>
+        <v>1.3247841965674459E-6</v>
+      </c>
+      <c r="C11" s="4">
+        <f>(B10-B11)/B10</f>
+        <v>-0.14214046453058282</v>
+      </c>
+      <c r="D11" s="4">
+        <f>(B2-B11)/B2</f>
+        <v>0.99124014278619477</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="31.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3">
+        <f>Subsumes8!B14</f>
+        <v>1.1247481090604601E-6</v>
+      </c>
+      <c r="C12" s="4">
+        <f>(B11-B12)/B11</f>
+        <v>0.15099522475078209</v>
+      </c>
+      <c r="D12" s="4">
+        <f>(B2-B12)/B2</f>
+        <v>0.99256283939497814</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="5">
+        <f>Subsumes8!B22</f>
+        <v>15</v>
+      </c>
+      <c r="H12" s="5">
+        <f>Subsumes8!C22</f>
+        <v>14</v>
+      </c>
+      <c r="I12" s="5">
+        <f>Subsumes8!D22</f>
+        <v>39</v>
+      </c>
+      <c r="J12" s="5">
+        <f>Subsumes8!E22</f>
+        <v>76</v>
+      </c>
+      <c r="K12" s="5">
+        <f>Subsumes8!F22</f>
+        <v>154</v>
+      </c>
+      <c r="L12" s="5">
+        <f>Subsumes8!G22</f>
+        <v>278</v>
+      </c>
+      <c r="M12" s="5">
+        <f>Subsumes8!H22</f>
+        <v>341</v>
+      </c>
+      <c r="N12" s="5">
+        <f>Subsumes8!I22</f>
+        <v>287</v>
+      </c>
+      <c r="O12" s="5">
+        <f>Subsumes8!J22</f>
+        <v>187</v>
+      </c>
+      <c r="P12" s="5">
+        <f>Subsumes8!K22</f>
+        <v>69</v>
+      </c>
+      <c r="Q12" s="5">
+        <f>Subsumes8!L22</f>
+        <v>14</v>
+      </c>
+      <c r="R12" s="5">
+        <f>Subsumes8!M22</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+      <c r="G13" s="7">
+        <f>(G7-G12)/G7</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" ref="H13:R13" si="3">(H7-H12)/H7</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="3"/>
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.17204301075268819</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.21690140845070421</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.25382932166301969</v>
+      </c>
+      <c r="N13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.2486910994764398</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.2723735408560311</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="Q13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3">
+        <f>Subsumes9!B14</f>
+        <v>9.6190895272287986E-7</v>
+      </c>
+      <c r="C14" s="4">
+        <f>(B12-B14)/B12</f>
+        <v>0.14477833305592774</v>
+      </c>
+      <c r="D14" s="4">
+        <f>(B2-B14)/B2</f>
+        <v>0.9936395791100423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -3346,11 +3983,24 @@
       </c>
       <c r="B11" s="2">
         <f>Subsumes8!P14</f>
-        <v>1.2648026325977652E-11</v>
+        <v>1.0273223719732067E-11</v>
       </c>
       <c r="C11" s="4">
         <f>(B10-B11)/B10</f>
-        <v>0.34728303608233102</v>
+        <v>0.46983764714197945</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2">
+        <f>Subsumes9!P14</f>
+        <v>1.0140610654526572E-11</v>
+      </c>
+      <c r="C12" s="4">
+        <f>(B11-B12)/B11</f>
+        <v>1.2908612605289813E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3399,14 +4049,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -3584,14 +4234,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -3620,14 +4270,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -3762,14 +4412,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -3947,14 +4597,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -3983,14 +4633,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -4151,24 +4801,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -4506,14 +5156,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -4542,14 +5192,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -4723,30 +5373,30 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="O2" s="33" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="O2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -5217,30 +5867,30 @@
       <c r="T15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="H16" s="33" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="H16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="O16" s="33" t="s">
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="O16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -5333,28 +5983,28 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5366,7 +6016,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="I14 B14 P14">
+  <conditionalFormatting sqref="B14 I14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5449,24 +6099,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -5839,14 +6489,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -5875,21 +6525,21 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -6051,24 +6701,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -6441,14 +7091,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -6477,24 +7127,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -6594,8 +7244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6656,24 +7306,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
@@ -6695,15 +7345,15 @@
         <v>1.4305686902419853E+21</v>
       </c>
       <c r="P3" s="26">
-        <v>18369507841</v>
+        <v>17994091157</v>
       </c>
       <c r="Q3" s="14">
         <f>P3/1000000000</f>
-        <v>18.369507841000001</v>
+        <v>17.994091157</v>
       </c>
       <c r="R3" s="14">
         <f>Q3/60</f>
-        <v>0.30615846401666669</v>
+        <v>0.29990151928333331</v>
       </c>
       <c r="S3" s="15"/>
       <c r="T3" s="15"/>
@@ -6723,15 +7373,15 @@
       <c r="F4" s="15"/>
       <c r="O4" s="32"/>
       <c r="P4" s="26">
-        <v>18373867338</v>
+        <v>15313024413</v>
       </c>
       <c r="Q4" s="14">
         <f t="shared" ref="Q4:Q7" si="1">P4/1000000000</f>
-        <v>18.373867338</v>
+        <v>15.313024413000001</v>
       </c>
       <c r="R4" s="14">
         <f>Q4/60</f>
-        <v>0.30623112229999999</v>
+        <v>0.25521707355000001</v>
       </c>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
@@ -6751,15 +7401,15 @@
       <c r="F5" s="15"/>
       <c r="O5" s="32"/>
       <c r="P5" s="26">
-        <v>18190809730</v>
+        <v>1790772636</v>
       </c>
       <c r="Q5" s="14">
         <f t="shared" si="1"/>
-        <v>18.190809730000002</v>
+        <v>1.790772636</v>
       </c>
       <c r="R5" s="14">
         <f>Q5/60</f>
-        <v>0.30318016216666671</v>
+        <v>2.9846210599999999E-2</v>
       </c>
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
@@ -6779,15 +7429,15 @@
       <c r="F6" s="15"/>
       <c r="O6" s="32"/>
       <c r="P6" s="26">
-        <v>18452816908</v>
+        <v>18086386139</v>
       </c>
       <c r="Q6" s="14">
         <f t="shared" si="1"/>
-        <v>18.452816907999999</v>
+        <v>18.086386138999998</v>
       </c>
       <c r="R6" s="14">
         <f t="shared" ref="R6:R11" si="2">Q6/60</f>
-        <v>0.30754694846666664</v>
+        <v>0.3014397689833333</v>
       </c>
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
@@ -6807,15 +7457,15 @@
       <c r="F7" s="15"/>
       <c r="O7" s="32"/>
       <c r="P7" s="26">
-        <v>18509145633</v>
+        <v>15698997206</v>
       </c>
       <c r="Q7" s="14">
         <f t="shared" si="1"/>
-        <v>18.509145632999999</v>
+        <v>15.698997206</v>
       </c>
       <c r="R7" s="14">
         <f t="shared" si="2"/>
-        <v>0.30848576054999999</v>
+        <v>0.2616499534333333</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
@@ -6863,15 +7513,15 @@
       <c r="F9" s="15"/>
       <c r="O9" s="15"/>
       <c r="P9" s="26">
-        <v>18381260627</v>
+        <v>17971904405</v>
       </c>
       <c r="Q9" s="14">
         <f>P9/1000000000</f>
-        <v>18.381260627</v>
+        <v>17.971904405</v>
       </c>
       <c r="R9" s="14">
         <f t="shared" si="2"/>
-        <v>0.30635434378333332</v>
+        <v>0.29953174008333333</v>
       </c>
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
@@ -6891,15 +7541,15 @@
       <c r="F10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="26">
-        <v>18285798148</v>
+        <v>14563143285</v>
       </c>
       <c r="Q10" s="14">
         <f t="shared" ref="Q10:Q14" si="4">P10/1000000000</f>
-        <v>18.285798148000001</v>
+        <v>14.563143285000001</v>
       </c>
       <c r="R10" s="14">
         <f t="shared" si="2"/>
-        <v>0.30476330246666666</v>
+        <v>0.24271905475000002</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
@@ -6919,15 +7569,15 @@
       <c r="F11" s="15"/>
       <c r="O11" s="15"/>
       <c r="P11" s="26">
-        <v>18430679818</v>
+        <v>14964804151</v>
       </c>
       <c r="Q11" s="14">
         <f t="shared" si="4"/>
-        <v>18.430679818000002</v>
+        <v>14.964804150999999</v>
       </c>
       <c r="R11" s="14">
         <f t="shared" si="2"/>
-        <v>0.3071779969666667</v>
+        <v>0.24941340251666666</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
@@ -6947,15 +7597,15 @@
       <c r="F12" s="15"/>
       <c r="O12" s="17"/>
       <c r="P12" s="27">
-        <v>18203873256</v>
+        <v>14841453367</v>
       </c>
       <c r="Q12" s="19">
         <f t="shared" si="4"/>
-        <v>18.203873256000001</v>
+        <v>14.841453367</v>
       </c>
       <c r="R12" s="19">
         <f>Q12/60</f>
-        <v>0.30339788760000003</v>
+        <v>0.24735755611666665</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
@@ -6983,19 +7633,19 @@
       </c>
       <c r="P13" s="20">
         <f>AVERAGE(P3:P12)</f>
-        <v>18093870455.299999</v>
+        <v>14696552201.299999</v>
       </c>
       <c r="Q13" s="21">
         <f t="shared" si="4"/>
-        <v>18.093870455299999</v>
+        <v>14.696552201299999</v>
       </c>
       <c r="R13" s="21">
         <f>Q13/60</f>
-        <v>0.30156450758833331</v>
+        <v>0.24494253668833332</v>
       </c>
       <c r="S13" s="21">
         <f>R13/60</f>
-        <v>5.0260751264722221E-3</v>
+        <v>4.0823756114722219E-3</v>
       </c>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
@@ -7020,19 +7670,19 @@
       </c>
       <c r="P14" s="26">
         <f>P13/O3</f>
-        <v>1.2648026325977652E-11</v>
+        <v>1.0273223719732067E-11</v>
       </c>
       <c r="Q14" s="23">
         <f t="shared" si="4"/>
-        <v>1.2648026325977651E-20</v>
+        <v>1.0273223719732067E-20</v>
       </c>
       <c r="R14" s="23">
         <f>Q14/60</f>
-        <v>2.1080043876629418E-22</v>
+        <v>1.7122039532886779E-22</v>
       </c>
       <c r="S14" s="15">
         <f>R14/60</f>
-        <v>3.5133406461049027E-24</v>
+        <v>2.8536732554811297E-24</v>
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
@@ -7046,14 +7696,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
@@ -7082,24 +7732,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -7115,31 +7765,31 @@
         <v>39</v>
       </c>
       <c r="E22" s="11">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F22" s="11">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="G22" s="11">
-        <v>355</v>
+        <v>278</v>
       </c>
       <c r="H22" s="11">
-        <v>457</v>
+        <v>341</v>
       </c>
       <c r="I22" s="11">
-        <v>382</v>
+        <v>287</v>
       </c>
       <c r="J22" s="11">
-        <v>257</v>
+        <v>187</v>
       </c>
       <c r="K22" s="11">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="L22" s="11">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M22" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.25">
@@ -7162,10 +7812,10 @@
         <v>36</v>
       </c>
       <c r="G23" s="11">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" s="11">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I23" s="11">
         <v>44</v>
@@ -7197,509 +7847,615 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" style="2"/>
-    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="11"/>
+    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="H2" s="25"/>
+      <c r="O2" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <f>15^12</f>
+        <v>129746337890625</v>
+      </c>
+      <c r="B3" s="13">
+        <f>123026876+2854569</f>
+        <v>125881445</v>
+      </c>
+      <c r="C3" s="14">
+        <f>B3/1000000000</f>
+        <v>0.12588144500000001</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="O3" s="12">
+        <f>21^16</f>
+        <v>1.4305686902419853E+21</v>
+      </c>
+      <c r="P3" s="26">
+        <v>14579866877</v>
+      </c>
+      <c r="Q3" s="14">
+        <f>P3/1000000000</f>
+        <v>14.579866877000001</v>
+      </c>
+      <c r="R3" s="14">
+        <f>Q3/60</f>
+        <v>0.24299778128333335</v>
+      </c>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
+      <c r="B4" s="13">
+        <f>119767133+2854569</f>
+        <v>122621702</v>
+      </c>
+      <c r="C4" s="14">
+        <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
+        <v>0.122621702</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="26">
+        <v>13279680567</v>
+      </c>
+      <c r="Q4" s="14">
+        <f t="shared" ref="Q4:Q7" si="1">P4/1000000000</f>
+        <v>13.279680567</v>
+      </c>
+      <c r="R4" s="14">
+        <f>Q4/60</f>
+        <v>0.22132800945</v>
+      </c>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="33"/>
+      <c r="B5" s="13">
+        <f>123209166+2854569</f>
+        <v>126063735</v>
+      </c>
+      <c r="C5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12606373500000001</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="26">
+        <v>14636515323</v>
+      </c>
+      <c r="Q5" s="14">
+        <f t="shared" si="1"/>
+        <v>14.636515322999999</v>
+      </c>
+      <c r="R5" s="14">
+        <f>Q5/60</f>
+        <v>0.24394192204999998</v>
+      </c>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="33"/>
+      <c r="B6" s="13">
+        <f>120883998+2854569</f>
+        <v>123738567</v>
+      </c>
+      <c r="C6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12373856699999999</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="26">
+        <v>14619739266</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="1"/>
+        <v>14.619739266</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" ref="R6:R11" si="2">Q6/60</f>
+        <v>0.2436623211</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="33"/>
+      <c r="B7" s="13">
+        <f>122830445+2854569</f>
+        <v>125685014</v>
+      </c>
+      <c r="C7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12568501400000001</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="26">
+        <v>14722877242</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="1"/>
+        <v>14.722877241999999</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="2"/>
+        <v>0.24538128736666664</v>
+      </c>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="13">
+        <f>121130362+2854569</f>
+        <v>123984931</v>
+      </c>
+      <c r="C8" s="14">
+        <f>B8/1000000000</f>
+        <v>0.12398493100000001</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="26">
+        <v>14630758711</v>
+      </c>
+      <c r="Q8" s="14">
+        <f>P8/1000000000</f>
+        <v>14.630758711</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="2"/>
+        <v>0.24384597851666667</v>
+      </c>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="13">
+        <f>122191452+2854569</f>
+        <v>125046021</v>
+      </c>
+      <c r="C9" s="14">
+        <f>B9/1000000000</f>
+        <v>0.12504602100000001</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="26">
+        <v>14557717725</v>
+      </c>
+      <c r="Q9" s="14">
+        <f>P9/1000000000</f>
+        <v>14.557717725</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="2"/>
+        <v>0.24262862874999999</v>
+      </c>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="13">
+        <f>122786257+2854569</f>
+        <v>125640826</v>
+      </c>
+      <c r="C10" s="14">
+        <f t="shared" ref="C10:C14" si="3">B10/1000000000</f>
+        <v>0.12564082600000001</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="26">
+        <v>14632654673</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" ref="Q10:Q14" si="4">P10/1000000000</f>
+        <v>14.632654672999999</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="2"/>
+        <v>0.24387757788333334</v>
+      </c>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="13">
+        <f>122993444+2854569</f>
+        <v>125848013</v>
+      </c>
+      <c r="C11" s="14">
+        <f t="shared" si="3"/>
+        <v>0.12584801300000001</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="26">
+        <v>14734461479</v>
+      </c>
+      <c r="Q11" s="14">
+        <f t="shared" si="4"/>
+        <v>14.734461479</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" si="2"/>
+        <v>0.24557435798333332</v>
+      </c>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18">
+        <f>120676817+2854569</f>
+        <v>123531386</v>
+      </c>
+      <c r="C12" s="19">
+        <f t="shared" si="3"/>
+        <v>0.12353138600000001</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="27">
+        <v>14674129160</v>
+      </c>
+      <c r="Q12" s="19">
+        <f t="shared" si="4"/>
+        <v>14.67412916</v>
+      </c>
+      <c r="R12" s="19">
+        <f>Q12/60</f>
+        <v>0.24456881933333333</v>
+      </c>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="20">
+        <f>AVERAGE(B3:B12)</f>
+        <v>124804164</v>
+      </c>
+      <c r="C13" s="21">
+        <f t="shared" si="3"/>
+        <v>0.124804164</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="1"/>
+      <c r="O13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="20">
+        <f>AVERAGE(P3:P12)</f>
+        <v>14506840102.299999</v>
+      </c>
+      <c r="Q13" s="21">
+        <f t="shared" si="4"/>
+        <v>14.5068401023</v>
+      </c>
+      <c r="R13" s="21">
+        <f>Q13/60</f>
+        <v>0.24178066837166667</v>
+      </c>
+      <c r="S13" s="21">
+        <f>R13/60</f>
+        <v>4.0296778061944443E-3</v>
+      </c>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="22">
+        <f>B13/A3</f>
+        <v>9.6190895272287986E-7</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" si="3"/>
+        <v>9.6190895272287991E-16</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="O14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14" s="26">
+        <f>P13/O3</f>
+        <v>1.0140610654526572E-11</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" si="4"/>
+        <v>1.0140610654526571E-20</v>
+      </c>
+      <c r="R14" s="23">
+        <f>Q14/60</f>
+        <v>1.6901017757544284E-22</v>
+      </c>
+      <c r="S14" s="15">
+        <f>R14/60</f>
+        <v>2.8168362929240473E-24</v>
+      </c>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="12">
+        <f>(55^33)</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="B17" s="13">
+        <f>A17*$B$14</f>
+        <v>2.6007746305388222E+51</v>
+      </c>
+      <c r="C17" s="13">
+        <f>C14*A17</f>
+        <v>2.6007746305388224E+42</v>
+      </c>
+      <c r="D17" s="15">
+        <f>C17/(60*60)</f>
+        <v>7.2243739737189509E+38</v>
+      </c>
+      <c r="E17" s="15">
+        <f>D17/24</f>
+        <v>3.0101558223828962E+37</v>
+      </c>
+      <c r="F17" s="15">
+        <f>E17/365</f>
+        <v>8.247002253103825E+34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+    </row>
+    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="11">
+        <v>15</v>
+      </c>
+      <c r="C22" s="11">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3">
-        <f>Subsumes1!B14</f>
-        <v>1.5123353774301645E-4</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="D22" s="11">
+        <v>39</v>
+      </c>
+      <c r="E22" s="11">
+        <v>76</v>
+      </c>
+      <c r="F22" s="11">
+        <v>154</v>
+      </c>
+      <c r="G22" s="11">
+        <v>278</v>
+      </c>
+      <c r="H22" s="11">
+        <v>341</v>
+      </c>
+      <c r="I22" s="11">
+        <v>287</v>
+      </c>
+      <c r="J22" s="11">
+        <v>187</v>
+      </c>
+      <c r="K22" s="11">
+        <v>69</v>
+      </c>
+      <c r="L22" s="11">
+        <v>14</v>
+      </c>
+      <c r="M22" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="11">
+        <v>1</v>
+      </c>
+      <c r="C23" s="11">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11">
+        <v>7</v>
+      </c>
+      <c r="E23" s="11">
         <v>17</v>
       </c>
-      <c r="G2" s="5">
-        <f>Subsumes1!B22</f>
-        <v>15</v>
-      </c>
-      <c r="H2" s="5">
-        <f>Subsumes1!C22</f>
-        <v>15</v>
-      </c>
-      <c r="I2" s="5">
-        <f>Subsumes1!D22</f>
-        <v>45</v>
-      </c>
-      <c r="J2" s="5">
-        <f>Subsumes1!E22</f>
-        <v>105</v>
-      </c>
-      <c r="K2" s="5">
-        <f>Subsumes1!F22</f>
-        <v>255</v>
-      </c>
-      <c r="L2" s="5">
-        <f>Subsumes1!G22</f>
-        <v>540</v>
-      </c>
-      <c r="M2" s="5">
-        <f>Subsumes1!H22</f>
-        <v>795</v>
-      </c>
-      <c r="N2" s="5">
-        <f>Subsumes1!I22</f>
-        <v>795</v>
-      </c>
-      <c r="O2" s="5">
-        <f>Subsumes1!J22</f>
-        <v>660</v>
-      </c>
-      <c r="P2" s="5">
-        <f>Subsumes1!K22</f>
-        <v>345</v>
-      </c>
-      <c r="Q2" s="5">
-        <f>Subsumes1!L22</f>
-        <v>120</v>
-      </c>
-      <c r="R2" s="5">
-        <f>Subsumes1!M22</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3">
-        <f>Subsumes2!B14</f>
-        <v>1.1208736842005942E-4</v>
-      </c>
-      <c r="C3" s="4">
-        <f>(B2-B3)/B2</f>
-        <v>0.25884582154968927</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="F3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="5">
-        <f>Subsumes2!B22</f>
-        <v>15</v>
-      </c>
-      <c r="H3" s="5">
-        <f>Subsumes2!C22</f>
-        <v>14</v>
-      </c>
-      <c r="I3" s="5">
-        <f>Subsumes2!D22</f>
-        <v>39</v>
-      </c>
-      <c r="J3" s="5">
-        <f>Subsumes2!E22</f>
-        <v>84</v>
-      </c>
-      <c r="K3" s="5">
-        <f>Subsumes2!F22</f>
-        <v>186</v>
-      </c>
-      <c r="L3" s="5">
-        <f>Subsumes2!G22</f>
-        <v>355</v>
-      </c>
-      <c r="M3" s="5">
-        <f>Subsumes2!H22</f>
-        <v>457</v>
-      </c>
-      <c r="N3" s="5">
-        <f>Subsumes2!I22</f>
-        <v>382</v>
-      </c>
-      <c r="O3" s="5">
-        <f>Subsumes2!J22</f>
-        <v>257</v>
-      </c>
-      <c r="P3" s="5">
-        <f>Subsumes2!K22</f>
-        <v>100</v>
-      </c>
-      <c r="Q3" s="5">
-        <f>Subsumes2!L22</f>
-        <v>21</v>
-      </c>
-      <c r="R3" s="5">
-        <f>Subsumes2!M22</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
-      <c r="G4" s="7">
-        <f>ABS(G2-G3)/G2</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="7">
-        <f t="shared" ref="H4:R4" si="0">ABS(H2-H3)/H2</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.27058823529411763</v>
-      </c>
-      <c r="L4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.34259259259259262</v>
-      </c>
-      <c r="M4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.42515723270440253</v>
-      </c>
-      <c r="N4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.51949685534591195</v>
-      </c>
-      <c r="O4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.6106060606060606</v>
-      </c>
-      <c r="P4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.71014492753623193</v>
-      </c>
-      <c r="Q4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="R4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="3">
-        <f>Subsumes3!B14</f>
-        <v>1.0581533388767822E-4</v>
-      </c>
-      <c r="C5" s="4">
-        <f>(B3-B5)/B3</f>
-        <v>5.5956657924879416E-2</v>
-      </c>
-      <c r="D5" s="4">
-        <f>ABS(B2-B5)/B2</f>
-        <v>0.30031833238282835</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5">
-        <f>Subsumes3!B22</f>
-        <v>15</v>
-      </c>
-      <c r="H5" s="5">
-        <f>Subsumes3!C22</f>
-        <v>14</v>
-      </c>
-      <c r="I5" s="5">
-        <f>Subsumes3!D22</f>
-        <v>39</v>
-      </c>
-      <c r="J5" s="5">
-        <f>Subsumes3!E22</f>
-        <v>84</v>
-      </c>
-      <c r="K5" s="5">
-        <f>Subsumes3!F22</f>
-        <v>186</v>
-      </c>
-      <c r="L5" s="5">
-        <f>Subsumes3!G22</f>
-        <v>355</v>
-      </c>
-      <c r="M5" s="5">
-        <f>Subsumes3!H22</f>
-        <v>457</v>
-      </c>
-      <c r="N5" s="5">
-        <f>Subsumes3!I22</f>
-        <v>382</v>
-      </c>
-      <c r="O5" s="5">
-        <f>Subsumes3!J22</f>
-        <v>257</v>
-      </c>
-      <c r="P5" s="5">
-        <f>Subsumes3!K22</f>
-        <v>100</v>
-      </c>
-      <c r="Q5" s="5">
-        <f>Subsumes3!L22</f>
-        <v>21</v>
-      </c>
-      <c r="R5" s="5">
-        <f>Subsumes3!M22</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
-      <c r="G6" s="7">
-        <f>ABS(G3-G5)/G3</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <f t="shared" ref="H6:R6" si="1">ABS(H3-H5)/H3</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3">
-        <f>Subsumes4!B14</f>
-        <v>1.5749834390105394E-5</v>
-      </c>
-      <c r="C7" s="4">
-        <f>(B5-B7)/B5</f>
-        <v>0.85115735298984496</v>
-      </c>
-      <c r="D7" s="4">
-        <f>(B2-B7)/B2</f>
-        <v>0.89585752852738065</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="5">
-        <f>Subsumes4!B22</f>
-        <v>15</v>
-      </c>
-      <c r="H7" s="5">
-        <f>Subsumes4!C22</f>
-        <v>14</v>
-      </c>
-      <c r="I7" s="5">
-        <f>Subsumes4!D22</f>
-        <v>39</v>
-      </c>
-      <c r="J7" s="5">
-        <f>Subsumes4!E22</f>
-        <v>84</v>
-      </c>
-      <c r="K7" s="5">
-        <f>Subsumes4!F22</f>
-        <v>186</v>
-      </c>
-      <c r="L7" s="5">
-        <f>Subsumes4!G22</f>
-        <v>355</v>
-      </c>
-      <c r="M7" s="5">
-        <f>Subsumes4!H22</f>
-        <v>457</v>
-      </c>
-      <c r="N7" s="5">
-        <f>Subsumes4!I22</f>
-        <v>382</v>
-      </c>
-      <c r="O7" s="5">
-        <f>Subsumes4!J22</f>
-        <v>257</v>
-      </c>
-      <c r="P7" s="5">
-        <f>Subsumes4!K22</f>
-        <v>100</v>
-      </c>
-      <c r="Q7" s="5">
-        <f>Subsumes4!L22</f>
-        <v>21</v>
-      </c>
-      <c r="R7" s="5">
-        <f>Subsumes4!M22</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
-      <c r="G8" s="7">
-        <f>ABS(G5-G7)/G5</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <f t="shared" ref="H8:R8" si="2">ABS(H5-H7)/H5</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3">
-        <f>MIN(Subsumes5!B14,Subsumes5!I14,Subsumes5!P14)</f>
-        <v>1.5487632479415025E-5</v>
-      </c>
-      <c r="C9" s="4">
-        <f>(B7-B9)/B7</f>
-        <v>1.6647915412691134E-2</v>
-      </c>
-      <c r="D9" s="4">
-        <f>(B2-B9)/B2</f>
-        <v>0.89759128358332552</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="F23" s="11">
+        <v>36</v>
+      </c>
+      <c r="G23" s="11">
+        <v>52</v>
+      </c>
+      <c r="H23" s="11">
+        <v>51</v>
+      </c>
+      <c r="I23" s="11">
+        <v>44</v>
+      </c>
+      <c r="J23" s="11">
         <v>23</v>
       </c>
-      <c r="B10" s="3">
-        <f>Subsumes6!B14</f>
-        <v>1.1599135462834068E-6</v>
-      </c>
-      <c r="C10" s="4">
-        <f>(B9-B10)/B9</f>
-        <v>0.92510711060421436</v>
-      </c>
-      <c r="D10" s="4">
-        <f>(B2-B10)/B2</f>
-        <v>0.99233031532824156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="3">
-        <f>Subsumes7!B14</f>
-        <v>1.3247841965674459E-6</v>
-      </c>
-      <c r="C11" s="4">
-        <f>(B10-B11)/B10</f>
-        <v>-0.14214046453058282</v>
-      </c>
-      <c r="D11" s="4">
-        <f>(B2-B11)/B2</f>
-        <v>0.99124014278619477</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3">
-        <f>Subsumes8!B14</f>
-        <v>1.1247481090604601E-6</v>
-      </c>
-      <c r="C12" s="4">
-        <f>(B11-B12)/B11</f>
-        <v>0.15099522475078209</v>
-      </c>
-      <c r="D12" s="4">
-        <f>(B2-B12)/B2</f>
-        <v>0.99256283939497814</v>
+      <c r="K23" s="11">
+        <v>8</v>
+      </c>
+      <c r="L23" s="11">
+        <v>4</v>
+      </c>
+      <c r="M23" s="11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A19:P19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update grafiek time tests
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
     <sheet name="Grafiek6" sheetId="8" r:id="rId12"/>
     <sheet name="Grafiek7" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -212,13 +217,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="169" formatCode="0.0000%"/>
-    <numFmt numFmtId="170" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0000%"/>
+    <numFmt numFmtId="169" formatCode="0.0000000E+00"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -369,7 +374,7 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -377,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,7 +391,7 @@
     <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -398,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -409,16 +414,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -426,10 +431,10 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -437,7 +442,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -455,11 +460,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -512,7 +517,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -578,7 +583,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-BE"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -611,9 +616,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Samenvatting_6!$A$2:$A$3,Samenvatting_6!$A$5,Samenvatting_6!$A$7,Samenvatting_6!$A$9,Samenvatting_6!$A$10:$A$12)</c:f>
+              <c:f>(Samenvatting_6!$A$2:$A$3,Samenvatting_6!$A$5,Samenvatting_6!$A$7,Samenvatting_6!$A$9,Samenvatting_6!$A$10:$A$12,Samenvatting_6!$A$14)</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Subsumes 1</c:v>
                 </c:pt>
@@ -638,38 +643,44 @@
                 <c:pt idx="7">
                   <c:v>Subsumes 8</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>Subsumes 9</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Samenvatting_6!$B$2:$B$3,Samenvatting_6!$B$5,Samenvatting_6!$B$7,Samenvatting_6!$B$9,Samenvatting_6!$B$10:$B$12)</c:f>
+              <c:f>(Samenvatting_6!$B$2:$B$3,Samenvatting_6!$B$5,Samenvatting_6!$B$7,Samenvatting_6!$B$9,Samenvatting_6!$B$10:$B$12,Samenvatting_6!$B$14)</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.5123353774301645E-4</c:v>
+                  <c:v>0.000151233537743016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1208736842005942E-4</c:v>
+                  <c:v>0.000112087368420059</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0581533388767822E-4</c:v>
+                  <c:v>0.000105815333887678</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5749834390105394E-5</c:v>
+                  <c:v>1.57498343901054E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5487632479415025E-5</c:v>
+                  <c:v>1.5487632479415E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1599135462834068E-6</c:v>
+                  <c:v>1.15991354628341E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3247841965674459E-6</c:v>
+                  <c:v>1.32478419656745E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1247481090604601E-6</c:v>
+                  <c:v>1.12474810906046E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6190895272288E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,16 +696,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="44946176"/>
-        <c:axId val="44947712"/>
+        <c:axId val="-2120592336"/>
+        <c:axId val="-2120588320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44946176"/>
+        <c:axId val="-2120592336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -729,10 +740,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44947712"/>
+        <c:crossAx val="-2120588320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -740,11 +751,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44947712"/>
+        <c:axId val="-2120588320"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.55E-4"/>
-          <c:min val="0"/>
+          <c:logBase val="10.0"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -802,13 +812,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44946176"/>
+        <c:crossAx val="-2120592336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0000000000000001E-5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -860,7 +869,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -881,6 +890,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -906,7 +916,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -972,7 +982,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-BE"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -1005,9 +1015,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Samenvatting_7!$A$7,Samenvatting_7!$A$9:$A$11)</c:f>
+              <c:f>(Samenvatting_7!$A$7,Samenvatting_7!$A$9:$A$11,Samenvatting_7!$A$12)</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Subsumes 4</c:v>
                 </c:pt>
@@ -1020,26 +1030,32 @@
                 <c:pt idx="3">
                   <c:v>Subsumes 8</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Subsumes 9</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Samenvatting_7!$B$7,Samenvatting_7!$B$9:$B$11)</c:f>
+              <c:f>(Samenvatting_7!$B$7,Samenvatting_7!$B$9:$B$11,Samenvatting_7!$B$12)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000E+00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>9.5419548041935121E-10</c:v>
+                  <c:v>9.54195480419351E-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7567906277502009E-11</c:v>
+                  <c:v>1.7567906277502E-11</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>1.9377505144133226E-11</c:v>
+                  <c:v>1.93775051441332E-11</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1.0273223719732067E-11</c:v>
+                  <c:v>1.02732237197321E-11</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.01406106545266E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1055,16 +1071,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="44807296"/>
-        <c:axId val="44810240"/>
+        <c:axId val="-2120442960"/>
+        <c:axId val="-2120439680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44807296"/>
+        <c:axId val="-2120442960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1099,10 +1115,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44810240"/>
+        <c:crossAx val="-2120439680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1110,10 +1126,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44810240"/>
+        <c:axId val="-2120439680"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000001E-9"/>
+          <c:logBase val="10.0"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1171,13 +1187,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44807296"/>
+        <c:crossAx val="-2120442960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1E-10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1229,7 +1244,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2459,7 +2474,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2470,7 +2485,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2481,7 +2496,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6079191"/>
+    <xdr:ext cx="9313333" cy="6079537"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -2508,7 +2523,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300882" cy="6079191"/>
+    <xdr:ext cx="9313333" cy="6079537"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -2824,14 +2839,14 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -3183,23 +3198,23 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" style="2"/>
-    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="18" width="7.83203125" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -3259,7 +3274,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -3324,7 +3339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G4" s="7">
         <f>ABS(G2-G3)/G2</f>
         <v>0</v>
@@ -3374,7 +3389,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -3442,7 +3457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G6" s="7">
         <f>ABS(G3-G5)/G3</f>
         <v>0</v>
@@ -3492,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -3560,7 +3575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G8" s="7">
         <f>ABS(G5-G7)/G5</f>
         <v>0</v>
@@ -3610,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -3628,7 +3643,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -3645,7 +3660,7 @@
         <v>0.99233031532824156</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -3662,7 +3677,7 @@
         <v>0.99124014278619477</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="31.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -3730,7 +3745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G13" s="7">
         <f>(G7-G12)/G7</f>
         <v>0</v>
@@ -3780,7 +3795,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -3806,34 +3821,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" style="2"/>
-    <col min="7" max="18" width="7.85546875" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="18" width="7.83203125" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="3"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -3842,7 +3857,7 @@
       <c r="D3" s="4"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -3856,7 +3871,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -3865,7 +3880,7 @@
       <c r="D5" s="4"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="14.1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -3879,7 +3894,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" ht="30.95" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -3941,7 +3956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -3950,7 +3965,7 @@
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -3964,7 +3979,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -3977,7 +3992,7 @@
         <v>-0.10300594948805275</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="26.1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -3990,7 +4005,7 @@
         <v>0.46983764714197945</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -4016,16 +4031,16 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -4380,15 +4395,15 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -4743,20 +4758,20 @@
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -5303,17 +5318,17 @@
       <selection activeCell="A22" sqref="A22:T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="28" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" style="28" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -5982,7 +5997,7 @@
         <v>6.4429744790623529E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
         <v>28</v>
       </c>
@@ -6016,7 +6031,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14 I14 P14">
+  <conditionalFormatting sqref="I14 B14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6041,20 +6056,20 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -6524,7 +6539,7 @@
         <v>9.9446102487422776E+34</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>29</v>
       </c>
@@ -6643,20 +6658,20 @@
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -7126,7 +7141,7 @@
         <v>1.1358141769074102E+35</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>30</v>
       </c>
@@ -7248,20 +7263,20 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -7731,7 +7746,7 @@
         <v>9.64311659990151E+34</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>31</v>
       </c>
@@ -7850,23 +7865,23 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="11"/>
-    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="11"/>
+    <col min="15" max="15" width="12.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -8346,7 +8361,7 @@
         <v>8.247002253103825E+34</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Update time test sheet
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -454,9 +454,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -696,11 +693,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2120592336"/>
-        <c:axId val="-2120588320"/>
+        <c:axId val="-2105015056"/>
+        <c:axId val="-2103140640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2120592336"/>
+        <c:axId val="-2105015056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +740,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120588320"/>
+        <c:crossAx val="-2103140640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -751,7 +748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120588320"/>
+        <c:axId val="-2103140640"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="maxMin"/>
@@ -815,7 +812,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120592336"/>
+        <c:crossAx val="-2105015056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1071,11 +1068,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="-2120442960"/>
-        <c:axId val="-2120439680"/>
+        <c:axId val="-2104947248"/>
+        <c:axId val="-2104943952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2120442960"/>
+        <c:axId val="-2104947248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1115,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120439680"/>
+        <c:crossAx val="-2104943952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120439680"/>
+        <c:axId val="-2104943952"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="maxMin"/>
@@ -1190,7 +1187,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120442960"/>
+        <c:crossAx val="-2104947248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2474,7 +2471,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3821,7 +3818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -6031,7 +6028,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="I14 B14 P14">
+  <conditionalFormatting sqref="B14 I14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6655,7 +6652,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="A19" sqref="A19:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7142,24 +7139,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -7260,7 +7257,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="A19" sqref="A19:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7747,24 +7744,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -7865,7 +7862,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8362,24 +8359,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">

</xml_diff>

<commit_message>
Updated statistics on Subs10/11 (Subs10+)
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Grafiek6" sheetId="8" r:id="rId13"/>
     <sheet name="Grafiek7" sheetId="13" r:id="rId14"/>
     <sheet name="Recursive vs Iterative" sheetId="19" r:id="rId15"/>
-    <sheet name="permutationCount" sheetId="20" r:id="rId16"/>
+    <sheet name="Stats_sub10+" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -33,8 +33,138 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lemma 4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lemma 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lemma 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+# keer geen mogelijkheden gevonden bij opstellen permutatie mogelijkheden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+# keer dat subsumes gecheckt wordt via permutaties.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="56">
   <si>
     <t>Tester</t>
   </si>
@@ -239,6 +369,42 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Subs11</t>
+  </si>
+  <si>
+    <t>uniqueC</t>
+  </si>
+  <si>
+    <t>redundantC</t>
+  </si>
+  <si>
+    <t>kLengthC</t>
+  </si>
+  <si>
+    <t>pLengthC</t>
+  </si>
+  <si>
+    <t>lLengthC</t>
+  </si>
+  <si>
+    <t>emptyPosC</t>
+  </si>
+  <si>
+    <t>Channel: 7</t>
+  </si>
+  <si>
+    <t>Channel 8</t>
+  </si>
+  <si>
+    <t>Subs11_ch7</t>
+  </si>
+  <si>
+    <t>Subs11_ch8</t>
+  </si>
+  <si>
+    <t>networkPC</t>
+  </si>
 </sst>
 </file>
 
@@ -252,9 +418,9 @@
     <numFmt numFmtId="168" formatCode="0.00000E+00"/>
     <numFmt numFmtId="169" formatCode="0.0000%"/>
     <numFmt numFmtId="170" formatCode="0.0000000E+00"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +520,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -482,6 +661,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -490,13 +676,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -531,7 +710,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -736,11 +914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="105034496"/>
-        <c:axId val="105037184"/>
+        <c:axId val="91870336"/>
+        <c:axId val="98676736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105034496"/>
+        <c:axId val="91870336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +961,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105037184"/>
+        <c:crossAx val="98676736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -791,7 +969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105037184"/>
+        <c:axId val="98676736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="maxMin"/>
@@ -855,7 +1033,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105034496"/>
+        <c:crossAx val="91870336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1075,11 +1253,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="107928192"/>
-        <c:axId val="107959808"/>
+        <c:axId val="98696192"/>
+        <c:axId val="101349248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107928192"/>
+        <c:axId val="98696192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1300,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107959808"/>
+        <c:crossAx val="101349248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1130,7 +1308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107959808"/>
+        <c:axId val="101349248"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="maxMin"/>
@@ -1196,7 +1374,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107928192"/>
+        <c:crossAx val="98696192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2876,14 +3054,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -3059,14 +3237,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -3095,14 +3273,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -3267,24 +3445,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -3637,14 +3815,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -3673,24 +3851,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -4599,14 +4777,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4718,218 +4896,519 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="36" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="37">
         <v>25790</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="38">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="37">
+        <v>37</v>
+      </c>
+      <c r="E3" s="37">
+        <v>51</v>
+      </c>
+      <c r="F3" s="37">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="37">
+        <v>16759</v>
+      </c>
+      <c r="K3" s="37">
+        <v>502414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="37">
         <v>215373</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="38">
         <v>118</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="37">
+        <v>97</v>
+      </c>
+      <c r="E4" s="37">
+        <v>391</v>
+      </c>
+      <c r="F4" s="37">
+        <v>315</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="37">
+        <v>18300</v>
+      </c>
+      <c r="K4" s="37">
+        <v>505768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="37">
         <v>503800</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="38">
         <v>384</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="37">
+        <v>353</v>
+      </c>
+      <c r="E5" s="37">
+        <v>981</v>
+      </c>
+      <c r="F5" s="37">
+        <v>900</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="37">
+        <v>797568</v>
+      </c>
+      <c r="K5" s="37">
+        <v>5701110921</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="37">
         <v>2251745</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="38">
         <v>1440</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="37">
+        <v>1096</v>
+      </c>
+      <c r="E6" s="37">
+        <v>4377</v>
+      </c>
+      <c r="F6" s="37">
+        <v>3563</v>
+      </c>
+      <c r="I6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="37">
+        <v>240682</v>
+      </c>
+      <c r="K6" s="37">
+        <v>99302113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="37">
         <v>8579924</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="38">
         <v>4770</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="37">
+        <v>3375</v>
+      </c>
+      <c r="E7" s="37">
+        <v>14469</v>
+      </c>
+      <c r="F7" s="37">
+        <v>10266</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="37">
+        <v>230976</v>
+      </c>
+      <c r="K7" s="37">
+        <v>94328317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="37">
         <v>31671913</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="38">
         <v>15680</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="37">
+        <v>10836</v>
+      </c>
+      <c r="E8" s="37">
+        <v>61500</v>
+      </c>
+      <c r="F8" s="37">
+        <v>43905</v>
+      </c>
+      <c r="I8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="37">
+        <v>43625</v>
+      </c>
+      <c r="K8" s="37">
+        <v>9816233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="37">
         <v>92226735</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="38">
         <v>37685</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="37">
+        <v>25245</v>
+      </c>
+      <c r="E9" s="37">
+        <v>336527</v>
+      </c>
+      <c r="F9" s="37">
+        <v>222639</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="37">
+        <v>133539</v>
+      </c>
+      <c r="K9" s="37">
+        <v>24458873</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="37">
         <v>171395459</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="38">
         <v>52337</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="37">
+        <v>35701</v>
+      </c>
+      <c r="E10" s="37">
+        <v>1633676</v>
+      </c>
+      <c r="F10" s="37">
+        <v>1051351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="37">
         <v>142580363</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="38">
         <v>38652</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="37">
+        <v>26609</v>
+      </c>
+      <c r="E11" s="37">
+        <v>5899932</v>
+      </c>
+      <c r="F11" s="37">
+        <v>3795601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="37">
         <v>67432031</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="38">
         <v>14901</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="37">
+        <v>10270</v>
+      </c>
+      <c r="E12" s="37">
+        <v>11434070</v>
+      </c>
+      <c r="F12" s="37">
+        <v>7246611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="37">
         <v>20205767</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="38">
         <v>3278</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="37">
+        <v>2400</v>
+      </c>
+      <c r="E13" s="37">
+        <v>10160707</v>
+      </c>
+      <c r="F13" s="37">
+        <v>6498474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="37">
         <v>2587416</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="38">
         <v>515</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="37">
+        <v>405</v>
+      </c>
+      <c r="E14" s="37">
+        <v>4155480</v>
+      </c>
+      <c r="F14" s="37">
+        <v>2706996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="37">
         <v>37053</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="38">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="37">
+        <v>41</v>
+      </c>
+      <c r="E15" s="37">
+        <v>970933</v>
+      </c>
+      <c r="F15" s="37">
+        <v>639125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="40">
+      <c r="B16" s="37">
         <v>0</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="37">
+        <v>0</v>
+      </c>
+      <c r="E16" s="37">
+        <v>133572</v>
+      </c>
+      <c r="F16" s="37">
+        <v>88561</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="37">
         <v>0</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17" s="37">
+        <v>0</v>
+      </c>
+      <c r="E17" s="37">
+        <v>10299</v>
+      </c>
+      <c r="F17" s="37">
+        <v>7436</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="37">
+        <v>0</v>
+      </c>
+      <c r="C18" s="38">
+        <v>0</v>
+      </c>
+      <c r="D18" s="37">
+        <v>0</v>
+      </c>
+      <c r="E18" s="37">
+        <v>510</v>
+      </c>
+      <c r="F18" s="37">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="37">
+        <v>0</v>
+      </c>
+      <c r="C19" s="38">
+        <v>0</v>
+      </c>
+      <c r="D19" s="37">
+        <v>0</v>
+      </c>
+      <c r="E19" s="37">
+        <v>14</v>
+      </c>
+      <c r="F19" s="37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="37">
+        <v>0</v>
+      </c>
+      <c r="C20" s="38">
+        <v>0</v>
+      </c>
+      <c r="D20" s="37">
+        <v>0</v>
+      </c>
+      <c r="E20" s="37">
+        <v>0</v>
+      </c>
+      <c r="F20" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="40">
-        <f>SUM(B3:B17)</f>
+      <c r="B21" s="37">
+        <f>SUM(B3:B20)</f>
         <v>539713369</v>
       </c>
-      <c r="C18" s="41">
-        <f>SUM(C3:C17)</f>
+      <c r="C21" s="38">
+        <f>SUM(C3:C20)</f>
         <v>169864</v>
       </c>
+      <c r="D21" s="38">
+        <f>SUM(D3:D20)</f>
+        <v>116465</v>
+      </c>
+      <c r="E21" s="38">
+        <f>SUM(E3:E20)</f>
+        <v>34817489</v>
+      </c>
+      <c r="F21" s="38">
+        <f>SUM(F3:F20)</f>
+        <v>22316193</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4974,14 +5453,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -5159,14 +5638,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -5195,14 +5674,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -5342,14 +5821,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -5527,14 +6006,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -5563,14 +6042,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -5736,24 +6215,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -6091,14 +6570,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -6127,14 +6606,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -6313,30 +6792,30 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="H2" s="36" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="H2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="O2" s="36" t="s">
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="O2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -6807,30 +7286,30 @@
       <c r="T15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="H16" s="36" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="H16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="O16" s="36" t="s">
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="O16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -6923,28 +7402,28 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6956,7 +7435,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14 I14 P14">
+  <conditionalFormatting sqref="I14 B14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -7044,24 +7523,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -7434,14 +7913,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -7470,21 +7949,21 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -7651,24 +8130,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -8041,14 +8520,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -8077,24 +8556,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -8261,24 +8740,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -8651,14 +9130,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -8687,24 +9166,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -8871,24 +9350,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -9271,14 +9750,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -9307,24 +9786,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">

</xml_diff>

<commit_message>
Added timetest subsumes11 + commented out permCount variable.
</commit_message>
<xml_diff>
--- a/timeTestPaper.xlsx
+++ b/timeTestPaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Subsumes1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,13 @@
     <sheet name="Subsumes8" sheetId="16" r:id="rId8"/>
     <sheet name="Subsumes9" sheetId="17" r:id="rId9"/>
     <sheet name="Subsumes10" sheetId="18" r:id="rId10"/>
-    <sheet name="Samenvatting_6" sheetId="6" r:id="rId11"/>
-    <sheet name="Samenvatting_7" sheetId="12" r:id="rId12"/>
-    <sheet name="Grafiek6" sheetId="8" r:id="rId13"/>
-    <sheet name="Grafiek7" sheetId="13" r:id="rId14"/>
-    <sheet name="Recursive vs Iterative" sheetId="19" r:id="rId15"/>
-    <sheet name="Stats_sub10+" sheetId="20" r:id="rId16"/>
+    <sheet name="Subsumes11" sheetId="21" r:id="rId11"/>
+    <sheet name="Samenvatting_6" sheetId="6" r:id="rId12"/>
+    <sheet name="Samenvatting_7" sheetId="12" r:id="rId13"/>
+    <sheet name="Grafiek6" sheetId="8" r:id="rId14"/>
+    <sheet name="Grafiek7" sheetId="13" r:id="rId15"/>
+    <sheet name="Recursive vs Iterative" sheetId="19" r:id="rId16"/>
+    <sheet name="Stats_sub10+" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -164,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="58">
   <si>
     <t>Tester</t>
   </si>
@@ -405,6 +406,12 @@
   <si>
     <t>networkPC</t>
   </si>
+  <si>
+    <t>Subsumes + Redundant Comparators + Permutation optilmalisation + Lemma 4 + test array/hash/… + Lemma 5 + Lemma 6 + PermRed + newUnique</t>
+  </si>
+  <si>
+    <t>Subsumes 11</t>
+  </si>
 </sst>
 </file>
 
@@ -561,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -578,6 +585,257 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -586,7 +844,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -664,9 +922,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -677,6 +934,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -914,11 +1213,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="91870336"/>
-        <c:axId val="98676736"/>
+        <c:axId val="104256640"/>
+        <c:axId val="104460288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91870336"/>
+        <c:axId val="104256640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -961,7 +1260,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98676736"/>
+        <c:crossAx val="104460288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -969,7 +1268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98676736"/>
+        <c:axId val="104460288"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="maxMin"/>
@@ -1033,7 +1332,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91870336"/>
+        <c:crossAx val="104256640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1191,9 +1490,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Samenvatting_7!$A$7,Samenvatting_7!$A$9:$A$13)</c:f>
+              <c:f>(Samenvatting_7!$A$7,Samenvatting_7!$A$9:$A$14)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Subsumes 4</c:v>
                 </c:pt>
@@ -1212,15 +1511,18 @@
                 <c:pt idx="5">
                   <c:v>Subsumes 10</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>Subsumes 11</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Samenvatting_7!$B$7,Samenvatting_7!$B$9:$B$13)</c:f>
+              <c:f>(Samenvatting_7!$B$7,Samenvatting_7!$B$9:$B$14)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000000E+00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>9.5419548041935121E-10</c:v>
                 </c:pt>
@@ -1239,6 +1541,9 @@
                 <c:pt idx="5" formatCode="General">
                   <c:v>5.2024658380724661E-13</c:v>
                 </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>3.2358931357689378E-13</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1253,11 +1558,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="98696192"/>
-        <c:axId val="101349248"/>
+        <c:axId val="104995840"/>
+        <c:axId val="105019264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98696192"/>
+        <c:axId val="104995840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1605,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101349248"/>
+        <c:crossAx val="105019264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1308,7 +1613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101349248"/>
+        <c:axId val="105019264"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="maxMin"/>
@@ -1374,7 +1679,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98696192"/>
+        <c:crossAx val="104995840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2669,7 +2974,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2707,7 +3012,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9301758" cy="6087070"/>
+    <xdr:ext cx="9300882" cy="6079191"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -3054,14 +3359,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -3237,14 +3542,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -3273,14 +3578,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -3384,7 +3689,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:P19"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,24 +3750,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -3815,14 +4120,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -3851,24 +4156,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -3898,6 +4203,519 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="11"/>
+    <col min="15" max="15" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="H2" s="25"/>
+      <c r="O2" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <f>15^12</f>
+        <v>129746337890625</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14">
+        <f>B3/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="O3" s="12">
+        <f>21^16</f>
+        <v>1.4305686902419853E+21</v>
+      </c>
+      <c r="P3" s="26">
+        <v>497704585</v>
+      </c>
+      <c r="Q3" s="14">
+        <f>P3/1000000000</f>
+        <v>0.49770458499999998</v>
+      </c>
+      <c r="R3" s="14">
+        <f>Q3/60</f>
+        <v>8.2950764166666666E-3</v>
+      </c>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14">
+        <f t="shared" ref="C4:C7" si="0">B4/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="26">
+        <v>451090850</v>
+      </c>
+      <c r="Q4" s="14">
+        <f t="shared" ref="Q4:Q7" si="1">P4/1000000000</f>
+        <v>0.45109084999999999</v>
+      </c>
+      <c r="R4" s="14">
+        <f>Q4/60</f>
+        <v>7.5181808333333331E-3</v>
+      </c>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="26">
+        <v>406611587</v>
+      </c>
+      <c r="Q5" s="14">
+        <f t="shared" si="1"/>
+        <v>0.406611587</v>
+      </c>
+      <c r="R5" s="14">
+        <f>Q5/60</f>
+        <v>6.7768597833333336E-3</v>
+      </c>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="26">
+        <v>482001999</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="1"/>
+        <v>0.48200199900000001</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" ref="R6:R11" si="2">Q6/60</f>
+        <v>8.0333666500000001E-3</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="26">
+        <v>414026374</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.41402637399999997</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="2"/>
+        <v>6.9004395666666662E-3</v>
+      </c>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14">
+        <f>B8/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="26">
+        <v>437945842</v>
+      </c>
+      <c r="Q8" s="14">
+        <f>P8/1000000000</f>
+        <v>0.43794584199999997</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="2"/>
+        <v>7.2990973666666658E-3</v>
+      </c>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14">
+        <f>B9/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="26">
+        <v>480518240</v>
+      </c>
+      <c r="Q9" s="14">
+        <f>P9/1000000000</f>
+        <v>0.48051823999999999</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="2"/>
+        <v>8.0086373333333339E-3</v>
+      </c>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14">
+        <f t="shared" ref="C10:C14" si="3">B10/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="26">
+        <v>480635189</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" ref="Q10:Q14" si="4">P10/1000000000</f>
+        <v>0.48063518900000002</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="2"/>
+        <v>8.0105864833333335E-3</v>
+      </c>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="26">
+        <v>458042853</v>
+      </c>
+      <c r="Q11" s="14">
+        <f t="shared" si="4"/>
+        <v>0.45804285300000003</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" si="2"/>
+        <v>7.6340475500000001E-3</v>
+      </c>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="27">
+        <v>520589886</v>
+      </c>
+      <c r="Q12" s="19">
+        <f t="shared" si="4"/>
+        <v>0.520589886</v>
+      </c>
+      <c r="R12" s="19">
+        <f>Q12/60</f>
+        <v>8.6764981000000008E-3</v>
+      </c>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="20" t="e">
+        <f>AVERAGE(B3:B12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="1"/>
+      <c r="O13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="20">
+        <f>AVERAGE(P3:P12)</f>
+        <v>462916740.5</v>
+      </c>
+      <c r="Q13" s="21">
+        <f t="shared" si="4"/>
+        <v>0.46291674049999998</v>
+      </c>
+      <c r="R13" s="21">
+        <f>Q13/60</f>
+        <v>7.7152790083333334E-3</v>
+      </c>
+      <c r="S13" s="21">
+        <f>R13/60</f>
+        <v>1.2858798347222222E-4</v>
+      </c>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="22" t="e">
+        <f>B13/A3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C14" s="23" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="O14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14" s="26">
+        <f>P13/O3</f>
+        <v>3.2358931357689378E-13</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" si="4"/>
+        <v>3.2358931357689378E-22</v>
+      </c>
+      <c r="R14" s="23">
+        <f>Q14/60</f>
+        <v>5.3931552262815631E-24</v>
+      </c>
+      <c r="S14" s="15">
+        <f>R14/60</f>
+        <v>8.9885920438026056E-26</v>
+      </c>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <f>(55^33)</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="B17" s="13" t="e">
+        <f>A17*$B$14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" s="13" t="e">
+        <f>C14*A17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" s="15" t="e">
+        <f>C17/(60*60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="15" t="e">
+        <f>D17/24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="15" t="e">
+        <f>E17/365</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+    </row>
+    <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A19:P19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
@@ -4537,12 +5355,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -4751,6 +5569,19 @@
         <v>0.94869672039178243</v>
       </c>
     </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="2">
+        <f>Subsumes11!$P$14</f>
+        <v>3.2358931357689378E-13</v>
+      </c>
+      <c r="C14" s="4">
+        <f>(B13-B14)/B13</f>
+        <v>0.3780078069733469</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4761,7 +5592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -4777,14 +5608,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4895,12 +5726,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4916,487 +5747,489 @@
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="41"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="F1" s="44"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="56"/>
+      <c r="B2" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2" s="50"/>
+      <c r="J2" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="57">
         <v>2</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="45">
         <v>25790</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="46">
         <v>37</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="46">
         <v>37</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="45">
         <v>51</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="47">
         <v>51</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="45">
         <v>16759</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="47">
         <v>502414</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="57">
         <v>3</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="45">
         <v>215373</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="46">
         <v>118</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="46">
         <v>97</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="45">
         <v>391</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="47">
         <v>315</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="45">
         <v>18300</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="47">
         <v>505768</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="57">
         <v>4</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="45">
         <v>503800</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="46">
         <v>384</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="46">
         <v>353</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="45">
         <v>981</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="47">
         <v>900</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="45">
         <v>797568</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="47">
         <v>5701110921</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="57">
         <v>5</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="45">
         <v>2251745</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="46">
         <v>1440</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="46">
         <v>1096</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="45">
         <v>4377</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="47">
         <v>3563</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="45">
         <v>240682</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="47">
         <v>99302113</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="57">
         <v>6</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="45">
         <v>8579924</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="46">
         <v>4770</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="46">
         <v>3375</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="45">
         <v>14469</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="47">
         <v>10266</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="45">
         <v>230976</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="47">
         <v>94328317</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="57">
         <v>7</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="45">
         <v>31671913</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="46">
         <v>15680</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="46">
         <v>10836</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="45">
         <v>61500</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="47">
         <v>43905</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="45">
         <v>43625</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="47">
         <v>9816233</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="57">
         <v>8</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="45">
         <v>92226735</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="46">
         <v>37685</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="46">
         <v>25245</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="45">
         <v>336527</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="47">
         <v>222639</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="48">
         <v>133539</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="49">
         <v>24458873</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="57">
         <v>9</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="45">
         <v>171395459</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="46">
         <v>52337</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="46">
         <v>35701</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="45">
         <v>1633676</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="47">
         <v>1051351</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="57">
         <v>10</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="45">
         <v>142580363</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="46">
         <v>38652</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="46">
         <v>26609</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="45">
         <v>5899932</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="47">
         <v>3795601</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="57">
         <v>11</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="45">
         <v>67432031</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="46">
         <v>14901</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="46">
         <v>10270</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="45">
         <v>11434070</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="47">
         <v>7246611</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="57">
         <v>12</v>
       </c>
-      <c r="B13" s="37">
+      <c r="B13" s="45">
         <v>20205767</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="46">
         <v>3278</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="46">
         <v>2400</v>
       </c>
-      <c r="E13" s="37">
+      <c r="E13" s="45">
         <v>10160707</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="47">
         <v>6498474</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="57">
         <v>13</v>
       </c>
-      <c r="B14" s="37">
+      <c r="B14" s="45">
         <v>2587416</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="46">
         <v>515</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="46">
         <v>405</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="45">
         <v>4155480</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="47">
         <v>2706996</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="57">
         <v>14</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="45">
         <v>37053</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="46">
         <v>67</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="46">
         <v>41</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="45">
         <v>970933</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="47">
         <v>639125</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="57">
         <v>15</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="45">
         <v>0</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="46">
         <v>0</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="46">
         <v>0</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="45">
         <v>133572</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="47">
         <v>88561</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="57">
         <v>16</v>
       </c>
-      <c r="B17" s="37">
+      <c r="B17" s="45">
         <v>0</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="46">
         <v>0</v>
       </c>
-      <c r="D17" s="37">
+      <c r="D17" s="46">
         <v>0</v>
       </c>
-      <c r="E17" s="37">
+      <c r="E17" s="45">
         <v>10299</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="47">
         <v>7436</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="57">
         <v>17</v>
       </c>
-      <c r="B18" s="37">
+      <c r="B18" s="45">
         <v>0</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="46">
         <v>0</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="46">
         <v>0</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="45">
         <v>510</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="47">
         <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="57">
         <v>18</v>
       </c>
-      <c r="B19" s="37">
+      <c r="B19" s="45">
         <v>0</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="46">
         <v>0</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D19" s="46">
         <v>0</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="45">
         <v>14</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F19" s="47">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="57">
         <v>19</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B20" s="45">
         <v>0</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="46">
         <v>0</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="46">
         <v>0</v>
       </c>
-      <c r="E20" s="37">
+      <c r="E20" s="45">
         <v>0</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="47">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="37">
+      <c r="B21" s="59">
         <f>SUM(B3:B20)</f>
         <v>539713369</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="60">
         <f>SUM(C3:C20)</f>
         <v>169864</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="60">
         <f>SUM(D3:D20)</f>
         <v>116465</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="60">
         <f>SUM(E3:E20)</f>
         <v>34817489</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="61">
         <f>SUM(F3:F20)</f>
         <v>22316193</v>
       </c>
@@ -5453,14 +6286,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -5638,14 +6471,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -5674,14 +6507,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -5821,14 +6654,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -6006,14 +6839,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -6042,14 +6875,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -6215,24 +7048,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -6570,14 +7403,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -6606,14 +7439,14 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -6792,30 +7625,30 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="H2" s="39" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="H2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="O2" s="39" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="O2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -7286,30 +8119,30 @@
       <c r="T15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="H16" s="39" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="H16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="O16" s="39" t="s">
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="O16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -7402,28 +8235,28 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="40"/>
-      <c r="T22" s="40"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7435,7 +8268,7 @@
     <mergeCell ref="O2:T2"/>
     <mergeCell ref="O16:T16"/>
   </mergeCells>
-  <conditionalFormatting sqref="I14 B14 P14">
+  <conditionalFormatting sqref="B14 I14 P14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -7523,24 +8356,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -7913,14 +8746,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -7949,21 +8782,21 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -8130,24 +8963,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -8520,14 +9353,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -8556,24 +9389,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -8740,24 +9573,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -9130,14 +9963,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -9166,24 +9999,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
@@ -9288,7 +10121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
@@ -9350,24 +10183,24 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="H2" s="25"/>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -9750,14 +10583,14 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -9786,24 +10619,24 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">

</xml_diff>